<commit_message>
Use the Guzzle HTTP client for object-oriented API code
</commit_message>
<xml_diff>
--- a/me/3.rest-restful-apis.xlsx
+++ b/me/3.rest-restful-apis.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BCC5C2-E7C6-49E0-8DFB-F2FDB3877889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71972EE-630D-43DE-BA1F-846B5097DA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REST and RESTful APIs" sheetId="1" r:id="rId1"/>
     <sheet name="Access a RESTful API" sheetId="2" r:id="rId2"/>
+    <sheet name="Guzzle HTTP" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="86">
   <si>
     <t>Method</t>
   </si>
@@ -276,6 +277,103 @@
       <t>",</t>
     </r>
   </si>
+  <si>
+    <t>github api</t>
+  </si>
+  <si>
+    <t>Personal access tokens</t>
+  </si>
+  <si>
+    <t>2.guzzlehttp</t>
+  </si>
+  <si>
+    <t>Guzzle HTTP code theo oop</t>
+  </si>
+  <si>
+    <t>install package bằng composer</t>
+  </si>
+  <si>
+    <t>composer require guzzlehttp/guzzle</t>
+  </si>
+  <si>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>composer.json</t>
+  </si>
+  <si>
+    <t>composer.lock</t>
+  </si>
+  <si>
+    <t>sau khi install package</t>
+  </si>
+  <si>
+    <t>rest-api-php\3.rest-and-restful-apis\2.guzzlehttp\index.php</t>
+  </si>
+  <si>
+    <t>require __DIR__ . "/vendor/autoload.php";</t>
+  </si>
+  <si>
+    <t>$client = new GuzzleHttp\Client;</t>
+  </si>
+  <si>
+    <t>$response = $client-&gt;request("GET", "https://api.github.com/user/repos", [</t>
+  </si>
+  <si>
+    <t>    "headers" =&gt; [</t>
+  </si>
+  <si>
+    <t>        "User-Agent" =&gt; "vudinhquang"</t>
+  </si>
+  <si>
+    <t>    ]</t>
+  </si>
+  <si>
+    <t>echo $response-&gt;getStatusCode(), "&lt;/br&gt;";</t>
+  </si>
+  <si>
+    <t>echo $response-&gt;getHeader("content-type")[0], "&lt;/br&gt;";</t>
+  </si>
+  <si>
+    <t>echo substr($response-&gt;getBody(), 0, 200), "...&lt;/br&gt;";</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        "Authorization" =&gt; "token </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>XXXXX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",</t>
+    </r>
+  </si>
+  <si>
+    <t>http://localhost/rest-api-php/3.rest-and-restful-apis/2.guzzlehttp/</t>
+  </si>
+  <si>
+    <t>Guzzle Documentation</t>
+  </si>
+  <si>
+    <t>https://docs.guzzlephp.org/en/stable/</t>
+  </si>
+  <si>
+    <t>Guzzle HTTP giúp code dễ đọc hơn dùng cURL</t>
+  </si>
 </sst>
 </file>
 
@@ -511,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -538,6 +636,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1001,6 +1109,557 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>423918</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBF7A99E-17EE-4D2D-8E45-9C3EF2874F75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752476" y="1476375"/>
+          <a:ext cx="11253842" cy="5705475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>74860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71EBAE51-BB92-443E-988C-2DFF2FF66944}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="7515225"/>
+          <a:ext cx="11106150" cy="5904160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>177772</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D09981B9-DBA2-4D31-817F-E80EC670FDA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="13773150"/>
+          <a:ext cx="11277600" cy="5464147"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>16661</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FC1B502-9AFE-442A-9859-E4598A8BFE5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="19535775"/>
+          <a:ext cx="11306175" cy="5636411"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>456259</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>189825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2002BEAD-D559-4386-AE19-AD6EBC229B7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="857250" y="25469850"/>
+          <a:ext cx="7523809" cy="5400000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>522938</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>104102</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B139A743-F95D-4D76-A321-89EB34163F4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="952500" y="31118175"/>
+          <a:ext cx="7495238" cy="5380952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>476251</xdr:colOff>
+      <xdr:row>216</xdr:row>
+      <xdr:rowOff>84743</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33C09E9F-ABEA-4A2B-80A2-07014438B59B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="781051" y="36737926"/>
+          <a:ext cx="11277600" cy="4504342"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>264</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>446409</xdr:colOff>
+      <xdr:row>293</xdr:row>
+      <xdr:rowOff>151700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECAB2084-4225-9EFE-7B0F-C4798A19E493}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="50387250"/>
+          <a:ext cx="10123809" cy="5600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>263</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>306</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBED61D1-6462-A1E7-D3F1-22E1E241FFEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="800100" y="50272950"/>
+          <a:ext cx="1647825" cy="8048625"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>335</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>208311</xdr:colOff>
+      <xdr:row>344</xdr:row>
+      <xdr:rowOff>114083</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C4DD651-2D20-A68D-7CB8-C080B24DB28D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="657225" y="63931800"/>
+          <a:ext cx="9914286" cy="1733333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>225</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>259</xdr:row>
+      <xdr:rowOff>79</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC907F1F-ADBF-7D2D-4941-353C484AF05D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="42976800"/>
+          <a:ext cx="11172825" cy="6381829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>321</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{629458AD-00BB-EA1B-6919-A736F1DC9B79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2676525" y="40176450"/>
+          <a:ext cx="1866900" cy="13611225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1339,8 +1998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE49C6D-7E2C-4616-9C87-29CAB5F475C1}">
   <dimension ref="A2:U208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="P59" sqref="P59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5150,4 +5809,3373 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1953F2BB-3AC0-4D47-A445-88716D13B605}">
+  <dimension ref="A2:U335"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
+      <selection activeCell="M326" sqref="M326"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="20"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="22"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="8"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="22"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="8"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="22"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="8"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="22"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="8"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="22"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="8"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="22"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="8"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="22"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="8"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="22"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="8"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="22"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="8"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="22"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="8"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="22"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="8"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="22"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="8"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="22"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+      <c r="B20" s="8"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="22"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="8"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="22"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="8"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="22"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="8"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="22"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="8"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="22"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="8"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="22"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
+      <c r="B26" s="8"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="22"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="21"/>
+      <c r="B27" s="8"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="22"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" s="8"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="22"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+      <c r="B29" s="8"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="22"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="21"/>
+      <c r="B30" s="8"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="22"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="21"/>
+      <c r="B31" s="8"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="22"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
+      <c r="B32" s="8"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="22"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="21"/>
+      <c r="B33" s="8"/>
+      <c r="T33" s="9"/>
+      <c r="U33" s="22"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="21"/>
+      <c r="B34" s="8"/>
+      <c r="T34" s="9"/>
+      <c r="U34" s="22"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="8"/>
+      <c r="T35" s="9"/>
+      <c r="U35" s="22"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="21"/>
+      <c r="B36" s="8"/>
+      <c r="T36" s="9"/>
+      <c r="U36" s="22"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="21"/>
+      <c r="B37" s="8"/>
+      <c r="T37" s="9"/>
+      <c r="U37" s="22"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+      <c r="B38" s="8"/>
+      <c r="T38" s="9"/>
+      <c r="U38" s="22"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="8"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="22"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="21"/>
+      <c r="B40" s="8"/>
+      <c r="T40" s="9"/>
+      <c r="U40" s="22"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="21"/>
+      <c r="B41" s="8"/>
+      <c r="T41" s="9"/>
+      <c r="U41" s="22"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="21"/>
+      <c r="B42" s="8"/>
+      <c r="T42" s="9"/>
+      <c r="U42" s="22"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+      <c r="B43" s="8"/>
+      <c r="T43" s="9"/>
+      <c r="U43" s="22"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="21"/>
+      <c r="B44" s="8"/>
+      <c r="T44" s="9"/>
+      <c r="U44" s="22"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" s="21"/>
+      <c r="B45" s="8"/>
+      <c r="T45" s="9"/>
+      <c r="U45" s="22"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="21"/>
+      <c r="B46" s="8"/>
+      <c r="T46" s="9"/>
+      <c r="U46" s="22"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="21"/>
+      <c r="B47" s="8"/>
+      <c r="T47" s="9"/>
+      <c r="U47" s="22"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" s="21"/>
+      <c r="B48" s="8"/>
+      <c r="T48" s="9"/>
+      <c r="U48" s="22"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" s="21"/>
+      <c r="B49" s="8"/>
+      <c r="T49" s="9"/>
+      <c r="U49" s="22"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50" s="21"/>
+      <c r="B50" s="8"/>
+      <c r="T50" s="9"/>
+      <c r="U50" s="22"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="B51" s="8"/>
+      <c r="T51" s="9"/>
+      <c r="U51" s="22"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" s="21"/>
+      <c r="B52" s="8"/>
+      <c r="T52" s="9"/>
+      <c r="U52" s="22"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A53" s="21"/>
+      <c r="B53" s="8"/>
+      <c r="T53" s="9"/>
+      <c r="U53" s="22"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A54" s="21"/>
+      <c r="B54" s="8"/>
+      <c r="T54" s="9"/>
+      <c r="U54" s="22"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A55" s="21"/>
+      <c r="B55" s="8"/>
+      <c r="T55" s="9"/>
+      <c r="U55" s="22"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A56" s="21"/>
+      <c r="B56" s="8"/>
+      <c r="T56" s="9"/>
+      <c r="U56" s="22"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A57" s="21"/>
+      <c r="B57" s="8"/>
+      <c r="T57" s="9"/>
+      <c r="U57" s="22"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A58" s="21"/>
+      <c r="B58" s="8"/>
+      <c r="T58" s="9"/>
+      <c r="U58" s="22"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A59" s="21"/>
+      <c r="B59" s="8"/>
+      <c r="T59" s="9"/>
+      <c r="U59" s="22"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A60" s="21"/>
+      <c r="B60" s="8"/>
+      <c r="T60" s="9"/>
+      <c r="U60" s="22"/>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A61" s="21"/>
+      <c r="B61" s="8"/>
+      <c r="T61" s="9"/>
+      <c r="U61" s="22"/>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A62" s="21"/>
+      <c r="B62" s="8"/>
+      <c r="T62" s="9"/>
+      <c r="U62" s="22"/>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A63" s="21"/>
+      <c r="B63" s="8"/>
+      <c r="T63" s="9"/>
+      <c r="U63" s="22"/>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A64" s="21"/>
+      <c r="B64" s="8"/>
+      <c r="T64" s="9"/>
+      <c r="U64" s="22"/>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A65" s="21"/>
+      <c r="B65" s="8"/>
+      <c r="T65" s="9"/>
+      <c r="U65" s="22"/>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A66" s="21"/>
+      <c r="B66" s="8"/>
+      <c r="T66" s="9"/>
+      <c r="U66" s="22"/>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A67" s="21"/>
+      <c r="B67" s="8"/>
+      <c r="T67" s="9"/>
+      <c r="U67" s="22"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A68" s="21"/>
+      <c r="B68" s="8"/>
+      <c r="T68" s="9"/>
+      <c r="U68" s="22"/>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A69" s="21"/>
+      <c r="B69" s="8"/>
+      <c r="T69" s="9"/>
+      <c r="U69" s="22"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A70" s="21"/>
+      <c r="B70" s="8"/>
+      <c r="T70" s="9"/>
+      <c r="U70" s="22"/>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A71" s="21"/>
+      <c r="B71" s="8"/>
+      <c r="T71" s="9"/>
+      <c r="U71" s="22"/>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A72" s="21"/>
+      <c r="B72" s="8"/>
+      <c r="T72" s="9"/>
+      <c r="U72" s="22"/>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A73" s="21"/>
+      <c r="B73" s="8"/>
+      <c r="T73" s="9"/>
+      <c r="U73" s="22"/>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A74" s="21"/>
+      <c r="B74" s="8"/>
+      <c r="T74" s="9"/>
+      <c r="U74" s="22"/>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A75" s="21"/>
+      <c r="B75" s="8"/>
+      <c r="T75" s="9"/>
+      <c r="U75" s="22"/>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A76" s="21"/>
+      <c r="B76" s="8"/>
+      <c r="T76" s="9"/>
+      <c r="U76" s="22"/>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A77" s="21"/>
+      <c r="B77" s="8"/>
+      <c r="T77" s="9"/>
+      <c r="U77" s="22"/>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A78" s="21"/>
+      <c r="B78" s="8"/>
+      <c r="T78" s="9"/>
+      <c r="U78" s="22"/>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A79" s="21"/>
+      <c r="B79" s="8"/>
+      <c r="T79" s="9"/>
+      <c r="U79" s="22"/>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A80" s="21"/>
+      <c r="B80" s="8"/>
+      <c r="T80" s="9"/>
+      <c r="U80" s="22"/>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A81" s="21"/>
+      <c r="B81" s="8"/>
+      <c r="T81" s="9"/>
+      <c r="U81" s="22"/>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A82" s="21"/>
+      <c r="B82" s="8"/>
+      <c r="T82" s="9"/>
+      <c r="U82" s="22"/>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A83" s="21"/>
+      <c r="B83" s="8"/>
+      <c r="T83" s="9"/>
+      <c r="U83" s="22"/>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A84" s="21"/>
+      <c r="B84" s="8"/>
+      <c r="T84" s="9"/>
+      <c r="U84" s="22"/>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A85" s="21"/>
+      <c r="B85" s="8"/>
+      <c r="T85" s="9"/>
+      <c r="U85" s="22"/>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A86" s="21"/>
+      <c r="B86" s="8"/>
+      <c r="T86" s="9"/>
+      <c r="U86" s="22"/>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A87" s="21"/>
+      <c r="B87" s="8"/>
+      <c r="T87" s="9"/>
+      <c r="U87" s="22"/>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A88" s="21"/>
+      <c r="B88" s="8"/>
+      <c r="T88" s="9"/>
+      <c r="U88" s="22"/>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A89" s="21"/>
+      <c r="B89" s="8"/>
+      <c r="T89" s="9"/>
+      <c r="U89" s="22"/>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A90" s="21"/>
+      <c r="B90" s="8"/>
+      <c r="T90" s="9"/>
+      <c r="U90" s="22"/>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A91" s="21"/>
+      <c r="B91" s="8"/>
+      <c r="T91" s="9"/>
+      <c r="U91" s="22"/>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A92" s="21"/>
+      <c r="B92" s="8"/>
+      <c r="T92" s="9"/>
+      <c r="U92" s="22"/>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A93" s="21"/>
+      <c r="B93" s="8"/>
+      <c r="T93" s="9"/>
+      <c r="U93" s="22"/>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A94" s="21"/>
+      <c r="B94" s="8"/>
+      <c r="T94" s="9"/>
+      <c r="U94" s="22"/>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A95" s="21"/>
+      <c r="B95" s="8"/>
+      <c r="T95" s="9"/>
+      <c r="U95" s="22"/>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A96" s="21"/>
+      <c r="B96" s="8"/>
+      <c r="T96" s="9"/>
+      <c r="U96" s="22"/>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A97" s="21"/>
+      <c r="B97" s="8"/>
+      <c r="T97" s="9"/>
+      <c r="U97" s="22"/>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A98" s="21"/>
+      <c r="B98" s="8"/>
+      <c r="T98" s="9"/>
+      <c r="U98" s="22"/>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A99" s="21"/>
+      <c r="B99" s="8"/>
+      <c r="T99" s="9"/>
+      <c r="U99" s="22"/>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A100" s="21"/>
+      <c r="B100" s="8"/>
+      <c r="T100" s="9"/>
+      <c r="U100" s="22"/>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A101" s="21"/>
+      <c r="B101" s="8"/>
+      <c r="T101" s="9"/>
+      <c r="U101" s="22"/>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A102" s="21"/>
+      <c r="B102" s="8"/>
+      <c r="T102" s="9"/>
+      <c r="U102" s="22"/>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A103" s="21"/>
+      <c r="B103" s="8"/>
+      <c r="T103" s="9"/>
+      <c r="U103" s="22"/>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A104" s="21"/>
+      <c r="B104" s="8"/>
+      <c r="T104" s="9"/>
+      <c r="U104" s="22"/>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A105" s="21"/>
+      <c r="B105" s="8"/>
+      <c r="T105" s="9"/>
+      <c r="U105" s="22"/>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A106" s="21"/>
+      <c r="B106" s="8"/>
+      <c r="T106" s="9"/>
+      <c r="U106" s="22"/>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A107" s="21"/>
+      <c r="B107" s="8"/>
+      <c r="T107" s="9"/>
+      <c r="U107" s="22"/>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A108" s="21"/>
+      <c r="B108" s="8"/>
+      <c r="T108" s="9"/>
+      <c r="U108" s="22"/>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A109" s="21"/>
+      <c r="B109" s="8"/>
+      <c r="T109" s="9"/>
+      <c r="U109" s="22"/>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A110" s="21"/>
+      <c r="B110" s="8"/>
+      <c r="T110" s="9"/>
+      <c r="U110" s="22"/>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A111" s="21"/>
+      <c r="B111" s="8"/>
+      <c r="T111" s="9"/>
+      <c r="U111" s="22"/>
+    </row>
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A112" s="21"/>
+      <c r="B112" s="8"/>
+      <c r="T112" s="9"/>
+      <c r="U112" s="22"/>
+    </row>
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A113" s="21"/>
+      <c r="B113" s="8"/>
+      <c r="T113" s="9"/>
+      <c r="U113" s="22"/>
+    </row>
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A114" s="21"/>
+      <c r="B114" s="8"/>
+      <c r="T114" s="9"/>
+      <c r="U114" s="22"/>
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A115" s="21"/>
+      <c r="B115" s="8"/>
+      <c r="T115" s="9"/>
+      <c r="U115" s="22"/>
+    </row>
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A116" s="21"/>
+      <c r="B116" s="8"/>
+      <c r="T116" s="9"/>
+      <c r="U116" s="22"/>
+    </row>
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A117" s="21"/>
+      <c r="B117" s="8"/>
+      <c r="T117" s="9"/>
+      <c r="U117" s="22"/>
+    </row>
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A118" s="21"/>
+      <c r="B118" s="8"/>
+      <c r="T118" s="9"/>
+      <c r="U118" s="22"/>
+    </row>
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A119" s="21"/>
+      <c r="B119" s="8"/>
+      <c r="T119" s="9"/>
+      <c r="U119" s="22"/>
+    </row>
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A120" s="21"/>
+      <c r="B120" s="8"/>
+      <c r="T120" s="9"/>
+      <c r="U120" s="22"/>
+    </row>
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A121" s="21"/>
+      <c r="B121" s="8"/>
+      <c r="T121" s="9"/>
+      <c r="U121" s="22"/>
+    </row>
+    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A122" s="21"/>
+      <c r="B122" s="8"/>
+      <c r="T122" s="9"/>
+      <c r="U122" s="22"/>
+    </row>
+    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A123" s="21"/>
+      <c r="B123" s="8"/>
+      <c r="T123" s="9"/>
+      <c r="U123" s="22"/>
+    </row>
+    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A124" s="21"/>
+      <c r="B124" s="8"/>
+      <c r="T124" s="9"/>
+      <c r="U124" s="22"/>
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A125" s="21"/>
+      <c r="B125" s="8"/>
+      <c r="T125" s="9"/>
+      <c r="U125" s="22"/>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A126" s="21"/>
+      <c r="B126" s="8"/>
+      <c r="T126" s="9"/>
+      <c r="U126" s="22"/>
+    </row>
+    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A127" s="21"/>
+      <c r="B127" s="8"/>
+      <c r="T127" s="9"/>
+      <c r="U127" s="22"/>
+    </row>
+    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A128" s="21"/>
+      <c r="B128" s="8"/>
+      <c r="T128" s="9"/>
+      <c r="U128" s="22"/>
+    </row>
+    <row r="129" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A129" s="21"/>
+      <c r="B129" s="8"/>
+      <c r="T129" s="9"/>
+      <c r="U129" s="22"/>
+    </row>
+    <row r="130" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A130" s="21"/>
+      <c r="B130" s="8"/>
+      <c r="T130" s="9"/>
+      <c r="U130" s="22"/>
+    </row>
+    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A131" s="21"/>
+      <c r="B131" s="8"/>
+      <c r="T131" s="9"/>
+      <c r="U131" s="22"/>
+    </row>
+    <row r="132" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A132" s="21"/>
+      <c r="B132" s="8"/>
+      <c r="T132" s="9"/>
+      <c r="U132" s="22"/>
+    </row>
+    <row r="133" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A133" s="21"/>
+      <c r="B133" s="8"/>
+      <c r="T133" s="9"/>
+      <c r="U133" s="22"/>
+    </row>
+    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A134" s="21"/>
+      <c r="B134" s="8"/>
+      <c r="T134" s="9"/>
+      <c r="U134" s="22"/>
+    </row>
+    <row r="135" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A135" s="21"/>
+      <c r="B135" s="8"/>
+      <c r="T135" s="9"/>
+      <c r="U135" s="22"/>
+    </row>
+    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A136" s="21"/>
+      <c r="B136" s="8"/>
+      <c r="T136" s="9"/>
+      <c r="U136" s="22"/>
+    </row>
+    <row r="137" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A137" s="21"/>
+      <c r="B137" s="8"/>
+      <c r="T137" s="9"/>
+      <c r="U137" s="22"/>
+    </row>
+    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A138" s="21"/>
+      <c r="B138" s="8"/>
+      <c r="T138" s="9"/>
+      <c r="U138" s="22"/>
+    </row>
+    <row r="139" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A139" s="21"/>
+      <c r="B139" s="8"/>
+      <c r="T139" s="9"/>
+      <c r="U139" s="22"/>
+    </row>
+    <row r="140" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A140" s="21"/>
+      <c r="B140" s="8"/>
+      <c r="T140" s="9"/>
+      <c r="U140" s="22"/>
+    </row>
+    <row r="141" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A141" s="21"/>
+      <c r="B141" s="8"/>
+      <c r="T141" s="9"/>
+      <c r="U141" s="22"/>
+    </row>
+    <row r="142" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A142" s="21"/>
+      <c r="B142" s="8"/>
+      <c r="T142" s="9"/>
+      <c r="U142" s="22"/>
+    </row>
+    <row r="143" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A143" s="21"/>
+      <c r="B143" s="8"/>
+      <c r="T143" s="9"/>
+      <c r="U143" s="22"/>
+    </row>
+    <row r="144" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A144" s="21"/>
+      <c r="B144" s="8"/>
+      <c r="T144" s="9"/>
+      <c r="U144" s="22"/>
+    </row>
+    <row r="145" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A145" s="21"/>
+      <c r="B145" s="8"/>
+      <c r="T145" s="9"/>
+      <c r="U145" s="22"/>
+    </row>
+    <row r="146" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A146" s="21"/>
+      <c r="B146" s="8"/>
+      <c r="T146" s="9"/>
+      <c r="U146" s="22"/>
+    </row>
+    <row r="147" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A147" s="21"/>
+      <c r="B147" s="8"/>
+      <c r="T147" s="9"/>
+      <c r="U147" s="22"/>
+    </row>
+    <row r="148" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A148" s="21"/>
+      <c r="B148" s="8"/>
+      <c r="T148" s="9"/>
+      <c r="U148" s="22"/>
+    </row>
+    <row r="149" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A149" s="21"/>
+      <c r="B149" s="8"/>
+      <c r="T149" s="9"/>
+      <c r="U149" s="22"/>
+    </row>
+    <row r="150" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A150" s="21"/>
+      <c r="B150" s="8"/>
+      <c r="T150" s="9"/>
+      <c r="U150" s="22"/>
+    </row>
+    <row r="151" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A151" s="21"/>
+      <c r="B151" s="8"/>
+      <c r="T151" s="9"/>
+      <c r="U151" s="22"/>
+    </row>
+    <row r="152" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A152" s="21"/>
+      <c r="B152" s="8"/>
+      <c r="T152" s="9"/>
+      <c r="U152" s="22"/>
+    </row>
+    <row r="153" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A153" s="21"/>
+      <c r="B153" s="8"/>
+      <c r="T153" s="9"/>
+      <c r="U153" s="22"/>
+    </row>
+    <row r="154" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A154" s="21"/>
+      <c r="B154" s="8"/>
+      <c r="T154" s="9"/>
+      <c r="U154" s="22"/>
+    </row>
+    <row r="155" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A155" s="21"/>
+      <c r="B155" s="8"/>
+      <c r="T155" s="9"/>
+      <c r="U155" s="22"/>
+    </row>
+    <row r="156" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A156" s="21"/>
+      <c r="B156" s="8"/>
+      <c r="T156" s="9"/>
+      <c r="U156" s="22"/>
+    </row>
+    <row r="157" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A157" s="21"/>
+      <c r="B157" s="8"/>
+      <c r="T157" s="9"/>
+      <c r="U157" s="22"/>
+    </row>
+    <row r="158" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A158" s="21"/>
+      <c r="B158" s="8"/>
+      <c r="T158" s="9"/>
+      <c r="U158" s="22"/>
+    </row>
+    <row r="159" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A159" s="21"/>
+      <c r="B159" s="8"/>
+      <c r="T159" s="9"/>
+      <c r="U159" s="22"/>
+    </row>
+    <row r="160" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A160" s="21"/>
+      <c r="B160" s="8"/>
+      <c r="T160" s="9"/>
+      <c r="U160" s="22"/>
+    </row>
+    <row r="161" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A161" s="21"/>
+      <c r="B161" s="8"/>
+      <c r="T161" s="9"/>
+      <c r="U161" s="22"/>
+    </row>
+    <row r="162" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A162" s="21"/>
+      <c r="B162" s="8"/>
+      <c r="T162" s="9"/>
+      <c r="U162" s="22"/>
+    </row>
+    <row r="163" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A163" s="21"/>
+      <c r="B163" s="8"/>
+      <c r="T163" s="9"/>
+      <c r="U163" s="22"/>
+    </row>
+    <row r="164" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A164" s="21"/>
+      <c r="B164" s="8"/>
+      <c r="T164" s="9"/>
+      <c r="U164" s="22"/>
+    </row>
+    <row r="165" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A165" s="21"/>
+      <c r="B165" s="8"/>
+      <c r="T165" s="9"/>
+      <c r="U165" s="22"/>
+    </row>
+    <row r="166" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A166" s="21"/>
+      <c r="B166" s="8"/>
+      <c r="T166" s="9"/>
+      <c r="U166" s="22"/>
+    </row>
+    <row r="167" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A167" s="21"/>
+      <c r="B167" s="8"/>
+      <c r="T167" s="9"/>
+      <c r="U167" s="22"/>
+    </row>
+    <row r="168" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A168" s="21"/>
+      <c r="B168" s="8"/>
+      <c r="T168" s="9"/>
+      <c r="U168" s="22"/>
+    </row>
+    <row r="169" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A169" s="21"/>
+      <c r="B169" s="8"/>
+      <c r="T169" s="9"/>
+      <c r="U169" s="22"/>
+    </row>
+    <row r="170" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A170" s="21"/>
+      <c r="B170" s="8"/>
+      <c r="T170" s="9"/>
+      <c r="U170" s="22"/>
+    </row>
+    <row r="171" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A171" s="21"/>
+      <c r="B171" s="8"/>
+      <c r="T171" s="9"/>
+      <c r="U171" s="22"/>
+    </row>
+    <row r="172" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A172" s="21"/>
+      <c r="B172" s="8"/>
+      <c r="T172" s="9"/>
+      <c r="U172" s="22"/>
+    </row>
+    <row r="173" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A173" s="21"/>
+      <c r="B173" s="8"/>
+      <c r="T173" s="9"/>
+      <c r="U173" s="22"/>
+    </row>
+    <row r="174" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A174" s="21"/>
+      <c r="B174" s="8"/>
+      <c r="T174" s="9"/>
+      <c r="U174" s="22"/>
+    </row>
+    <row r="175" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A175" s="21"/>
+      <c r="B175" s="8"/>
+      <c r="T175" s="9"/>
+      <c r="U175" s="22"/>
+    </row>
+    <row r="176" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A176" s="21"/>
+      <c r="B176" s="8"/>
+      <c r="T176" s="9"/>
+      <c r="U176" s="22"/>
+    </row>
+    <row r="177" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A177" s="21"/>
+      <c r="B177" s="8"/>
+      <c r="T177" s="9"/>
+      <c r="U177" s="22"/>
+    </row>
+    <row r="178" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A178" s="21"/>
+      <c r="B178" s="8"/>
+      <c r="T178" s="9"/>
+      <c r="U178" s="22"/>
+    </row>
+    <row r="179" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A179" s="21"/>
+      <c r="B179" s="8"/>
+      <c r="T179" s="9"/>
+      <c r="U179" s="22"/>
+    </row>
+    <row r="180" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A180" s="21"/>
+      <c r="B180" s="8"/>
+      <c r="T180" s="9"/>
+      <c r="U180" s="22"/>
+    </row>
+    <row r="181" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A181" s="21"/>
+      <c r="B181" s="8"/>
+      <c r="T181" s="9"/>
+      <c r="U181" s="22"/>
+    </row>
+    <row r="182" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A182" s="21"/>
+      <c r="B182" s="8"/>
+      <c r="T182" s="9"/>
+      <c r="U182" s="22"/>
+    </row>
+    <row r="183" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A183" s="21"/>
+      <c r="B183" s="8"/>
+      <c r="T183" s="9"/>
+      <c r="U183" s="22"/>
+    </row>
+    <row r="184" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A184" s="21"/>
+      <c r="B184" s="8"/>
+      <c r="T184" s="9"/>
+      <c r="U184" s="22"/>
+    </row>
+    <row r="185" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A185" s="21"/>
+      <c r="B185" s="8"/>
+      <c r="T185" s="9"/>
+      <c r="U185" s="22"/>
+    </row>
+    <row r="186" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A186" s="21"/>
+      <c r="B186" s="8"/>
+      <c r="T186" s="9"/>
+      <c r="U186" s="22"/>
+    </row>
+    <row r="187" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A187" s="21"/>
+      <c r="B187" s="8"/>
+      <c r="T187" s="9"/>
+      <c r="U187" s="22"/>
+    </row>
+    <row r="188" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A188" s="21"/>
+      <c r="B188" s="8"/>
+      <c r="T188" s="9"/>
+      <c r="U188" s="22"/>
+    </row>
+    <row r="189" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A189" s="21"/>
+      <c r="B189" s="8"/>
+      <c r="T189" s="9"/>
+      <c r="U189" s="22"/>
+    </row>
+    <row r="190" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A190" s="21"/>
+      <c r="B190" s="8"/>
+      <c r="T190" s="9"/>
+      <c r="U190" s="22"/>
+    </row>
+    <row r="191" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A191" s="21"/>
+      <c r="B191" s="8"/>
+      <c r="T191" s="9"/>
+      <c r="U191" s="22"/>
+    </row>
+    <row r="192" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A192" s="21"/>
+      <c r="B192" s="8"/>
+      <c r="T192" s="9"/>
+      <c r="U192" s="22"/>
+    </row>
+    <row r="193" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A193" s="21"/>
+      <c r="B193" s="8"/>
+      <c r="T193" s="9"/>
+      <c r="U193" s="22"/>
+    </row>
+    <row r="194" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A194" s="21"/>
+      <c r="B194" s="8"/>
+      <c r="T194" s="9"/>
+      <c r="U194" s="22"/>
+    </row>
+    <row r="195" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A195" s="21"/>
+      <c r="B195" s="8"/>
+      <c r="T195" s="9"/>
+      <c r="U195" s="22"/>
+    </row>
+    <row r="196" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A196" s="21"/>
+      <c r="B196" s="8"/>
+      <c r="T196" s="9"/>
+      <c r="U196" s="22"/>
+    </row>
+    <row r="197" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A197" s="21"/>
+      <c r="B197" s="8"/>
+      <c r="T197" s="9"/>
+      <c r="U197" s="22"/>
+    </row>
+    <row r="198" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A198" s="21"/>
+      <c r="B198" s="8"/>
+      <c r="T198" s="9"/>
+      <c r="U198" s="22"/>
+    </row>
+    <row r="199" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A199" s="21"/>
+      <c r="B199" s="8"/>
+      <c r="T199" s="9"/>
+      <c r="U199" s="22"/>
+    </row>
+    <row r="200" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A200" s="21"/>
+      <c r="B200" s="8"/>
+      <c r="T200" s="9"/>
+      <c r="U200" s="22"/>
+    </row>
+    <row r="201" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A201" s="21"/>
+      <c r="B201" s="8"/>
+      <c r="T201" s="9"/>
+      <c r="U201" s="22"/>
+    </row>
+    <row r="202" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A202" s="21"/>
+      <c r="B202" s="8"/>
+      <c r="T202" s="9"/>
+      <c r="U202" s="22"/>
+    </row>
+    <row r="203" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A203" s="21"/>
+      <c r="B203" s="8"/>
+      <c r="T203" s="9"/>
+      <c r="U203" s="22"/>
+    </row>
+    <row r="204" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A204" s="21"/>
+      <c r="B204" s="8"/>
+      <c r="T204" s="9"/>
+      <c r="U204" s="22"/>
+    </row>
+    <row r="205" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A205" s="21"/>
+      <c r="B205" s="8"/>
+      <c r="T205" s="9"/>
+      <c r="U205" s="22"/>
+    </row>
+    <row r="206" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A206" s="21"/>
+      <c r="B206" s="8"/>
+      <c r="T206" s="9"/>
+      <c r="U206" s="22"/>
+    </row>
+    <row r="207" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A207" s="21"/>
+      <c r="B207" s="8"/>
+      <c r="T207" s="9"/>
+      <c r="U207" s="22"/>
+    </row>
+    <row r="208" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A208" s="21"/>
+      <c r="B208" s="8"/>
+      <c r="T208" s="9"/>
+      <c r="U208" s="22"/>
+    </row>
+    <row r="209" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A209" s="21"/>
+      <c r="B209" s="8"/>
+      <c r="T209" s="9"/>
+      <c r="U209" s="22"/>
+    </row>
+    <row r="210" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A210" s="21"/>
+      <c r="B210" s="8"/>
+      <c r="T210" s="9"/>
+      <c r="U210" s="22"/>
+    </row>
+    <row r="211" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A211" s="21"/>
+      <c r="B211" s="8"/>
+      <c r="T211" s="9"/>
+      <c r="U211" s="22"/>
+    </row>
+    <row r="212" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A212" s="21"/>
+      <c r="B212" s="8"/>
+      <c r="T212" s="9"/>
+      <c r="U212" s="22"/>
+    </row>
+    <row r="213" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A213" s="21"/>
+      <c r="B213" s="8"/>
+      <c r="T213" s="9"/>
+      <c r="U213" s="22"/>
+    </row>
+    <row r="214" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A214" s="21"/>
+      <c r="B214" s="8"/>
+      <c r="T214" s="9"/>
+      <c r="U214" s="22"/>
+    </row>
+    <row r="215" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A215" s="21"/>
+      <c r="B215" s="8"/>
+      <c r="T215" s="9"/>
+      <c r="U215" s="22"/>
+    </row>
+    <row r="216" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A216" s="21"/>
+      <c r="B216" s="8"/>
+      <c r="T216" s="9"/>
+      <c r="U216" s="22"/>
+    </row>
+    <row r="217" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A217" s="21"/>
+      <c r="B217" s="8"/>
+      <c r="T217" s="9"/>
+      <c r="U217" s="22"/>
+    </row>
+    <row r="218" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A218" s="21"/>
+      <c r="B218" s="10"/>
+      <c r="C218" s="11"/>
+      <c r="D218" s="11"/>
+      <c r="E218" s="11"/>
+      <c r="F218" s="11"/>
+      <c r="G218" s="11"/>
+      <c r="H218" s="11"/>
+      <c r="I218" s="11"/>
+      <c r="J218" s="11"/>
+      <c r="K218" s="11"/>
+      <c r="L218" s="11"/>
+      <c r="M218" s="11"/>
+      <c r="N218" s="11"/>
+      <c r="O218" s="11"/>
+      <c r="P218" s="11"/>
+      <c r="Q218" s="11"/>
+      <c r="R218" s="11"/>
+      <c r="S218" s="11"/>
+      <c r="T218" s="13"/>
+      <c r="U218" s="22"/>
+    </row>
+    <row r="219" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A219" s="21"/>
+      <c r="U219" s="22"/>
+    </row>
+    <row r="220" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A220" s="21"/>
+      <c r="U220" s="22"/>
+    </row>
+    <row r="221" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="23"/>
+      <c r="B221" s="24"/>
+      <c r="C221" s="24"/>
+      <c r="D221" s="24"/>
+      <c r="E221" s="24"/>
+      <c r="F221" s="24"/>
+      <c r="G221" s="24"/>
+      <c r="H221" s="24"/>
+      <c r="I221" s="24"/>
+      <c r="J221" s="24"/>
+      <c r="K221" s="24"/>
+      <c r="L221" s="24"/>
+      <c r="M221" s="24"/>
+      <c r="N221" s="24"/>
+      <c r="O221" s="24"/>
+      <c r="P221" s="24"/>
+      <c r="Q221" s="24"/>
+      <c r="R221" s="24"/>
+      <c r="S221" s="24"/>
+      <c r="T221" s="24"/>
+      <c r="U221" s="25"/>
+    </row>
+    <row r="222" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A222" s="15"/>
+      <c r="B222" s="15"/>
+      <c r="C222" s="15"/>
+      <c r="D222" s="15"/>
+      <c r="E222" s="15"/>
+      <c r="F222" s="15"/>
+      <c r="G222" s="15"/>
+      <c r="H222" s="15"/>
+      <c r="I222" s="15"/>
+      <c r="J222" s="15"/>
+      <c r="K222" s="15"/>
+      <c r="L222" s="15"/>
+      <c r="M222" s="15"/>
+      <c r="N222" s="15"/>
+      <c r="O222" s="15"/>
+      <c r="P222" s="15"/>
+      <c r="Q222" s="15"/>
+      <c r="R222" s="15"/>
+      <c r="S222" s="15"/>
+      <c r="T222" s="15"/>
+      <c r="U222" s="15"/>
+    </row>
+    <row r="223" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A223" s="15"/>
+      <c r="B223" s="15"/>
+      <c r="C223" s="15"/>
+      <c r="D223" s="15"/>
+      <c r="E223" s="15"/>
+      <c r="F223" s="15"/>
+      <c r="G223" s="15"/>
+      <c r="H223" s="15"/>
+      <c r="I223" s="15"/>
+      <c r="J223" s="15"/>
+      <c r="K223" s="15"/>
+      <c r="L223" s="15"/>
+      <c r="M223" s="15"/>
+      <c r="N223" s="15"/>
+      <c r="O223" s="15"/>
+      <c r="P223" s="15"/>
+      <c r="Q223" s="15"/>
+      <c r="R223" s="15"/>
+      <c r="S223" s="15"/>
+      <c r="T223" s="15"/>
+      <c r="U223" s="15"/>
+    </row>
+    <row r="224" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A224" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B224" s="6"/>
+      <c r="C224" s="6"/>
+      <c r="D224" s="6"/>
+      <c r="E224" s="6"/>
+      <c r="F224" s="6"/>
+      <c r="G224" s="6"/>
+      <c r="H224" s="6"/>
+      <c r="I224" s="6"/>
+      <c r="J224" s="6"/>
+      <c r="K224" s="6"/>
+      <c r="L224" s="6"/>
+      <c r="M224" s="6"/>
+      <c r="N224" s="6"/>
+      <c r="O224" s="6"/>
+      <c r="P224" s="6"/>
+      <c r="Q224" s="6"/>
+      <c r="R224" s="6"/>
+      <c r="S224" s="6"/>
+      <c r="T224" s="7"/>
+      <c r="U224" s="15"/>
+    </row>
+    <row r="225" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A225" s="35"/>
+      <c r="B225" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C225" s="15"/>
+      <c r="D225" s="15"/>
+      <c r="E225" s="15"/>
+      <c r="F225" s="15"/>
+      <c r="G225" s="15"/>
+      <c r="H225" s="15"/>
+      <c r="I225" s="15"/>
+      <c r="J225" s="15"/>
+      <c r="K225" s="15"/>
+      <c r="L225" s="15"/>
+      <c r="M225" s="15"/>
+      <c r="N225" s="15"/>
+      <c r="O225" s="15"/>
+      <c r="P225" s="15"/>
+      <c r="Q225" s="15"/>
+      <c r="R225" s="15"/>
+      <c r="S225" s="15"/>
+      <c r="T225" s="9"/>
+      <c r="U225" s="15"/>
+    </row>
+    <row r="226" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A226" s="35"/>
+      <c r="B226" s="15"/>
+      <c r="C226" s="15"/>
+      <c r="D226" s="15"/>
+      <c r="E226" s="15"/>
+      <c r="F226" s="15"/>
+      <c r="G226" s="15"/>
+      <c r="H226" s="15"/>
+      <c r="I226" s="15"/>
+      <c r="J226" s="15"/>
+      <c r="K226" s="15"/>
+      <c r="L226" s="15"/>
+      <c r="M226" s="15"/>
+      <c r="N226" s="15"/>
+      <c r="O226" s="15"/>
+      <c r="P226" s="15"/>
+      <c r="Q226" s="15"/>
+      <c r="R226" s="15"/>
+      <c r="S226" s="15"/>
+      <c r="T226" s="9"/>
+      <c r="U226" s="15"/>
+    </row>
+    <row r="227" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A227" s="35"/>
+      <c r="B227" s="15"/>
+      <c r="C227" s="15"/>
+      <c r="D227" s="15"/>
+      <c r="E227" s="15"/>
+      <c r="F227" s="15"/>
+      <c r="G227" s="15"/>
+      <c r="H227" s="15"/>
+      <c r="I227" s="15"/>
+      <c r="J227" s="15"/>
+      <c r="K227" s="15"/>
+      <c r="L227" s="15"/>
+      <c r="M227" s="15"/>
+      <c r="N227" s="15"/>
+      <c r="O227" s="15"/>
+      <c r="P227" s="15"/>
+      <c r="Q227" s="15"/>
+      <c r="R227" s="15"/>
+      <c r="S227" s="15"/>
+      <c r="T227" s="9"/>
+      <c r="U227" s="15"/>
+    </row>
+    <row r="228" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A228" s="35"/>
+      <c r="B228" s="15"/>
+      <c r="C228" s="15"/>
+      <c r="D228" s="15"/>
+      <c r="E228" s="15"/>
+      <c r="F228" s="15"/>
+      <c r="G228" s="15"/>
+      <c r="H228" s="15"/>
+      <c r="I228" s="15"/>
+      <c r="J228" s="15"/>
+      <c r="K228" s="15"/>
+      <c r="L228" s="15"/>
+      <c r="M228" s="15"/>
+      <c r="N228" s="15"/>
+      <c r="O228" s="15"/>
+      <c r="P228" s="15"/>
+      <c r="Q228" s="15"/>
+      <c r="R228" s="15"/>
+      <c r="S228" s="15"/>
+      <c r="T228" s="9"/>
+      <c r="U228" s="15"/>
+    </row>
+    <row r="229" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A229" s="35"/>
+      <c r="B229" s="15"/>
+      <c r="C229" s="15"/>
+      <c r="D229" s="15"/>
+      <c r="E229" s="15"/>
+      <c r="F229" s="15"/>
+      <c r="G229" s="15"/>
+      <c r="H229" s="15"/>
+      <c r="I229" s="15"/>
+      <c r="J229" s="15"/>
+      <c r="K229" s="15"/>
+      <c r="L229" s="15"/>
+      <c r="M229" s="15"/>
+      <c r="N229" s="15"/>
+      <c r="O229" s="15"/>
+      <c r="P229" s="15"/>
+      <c r="Q229" s="15"/>
+      <c r="R229" s="15"/>
+      <c r="S229" s="15"/>
+      <c r="T229" s="9"/>
+      <c r="U229" s="15"/>
+    </row>
+    <row r="230" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A230" s="35"/>
+      <c r="B230" s="15"/>
+      <c r="C230" s="15"/>
+      <c r="D230" s="15"/>
+      <c r="E230" s="15"/>
+      <c r="F230" s="15"/>
+      <c r="G230" s="15"/>
+      <c r="H230" s="15"/>
+      <c r="I230" s="15"/>
+      <c r="J230" s="15"/>
+      <c r="K230" s="15"/>
+      <c r="L230" s="15"/>
+      <c r="M230" s="15"/>
+      <c r="N230" s="15"/>
+      <c r="O230" s="15"/>
+      <c r="P230" s="15"/>
+      <c r="Q230" s="15"/>
+      <c r="R230" s="15"/>
+      <c r="S230" s="15"/>
+      <c r="T230" s="9"/>
+      <c r="U230" s="15"/>
+    </row>
+    <row r="231" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A231" s="35"/>
+      <c r="B231" s="15"/>
+      <c r="C231" s="15"/>
+      <c r="D231" s="15"/>
+      <c r="E231" s="15"/>
+      <c r="F231" s="15"/>
+      <c r="G231" s="15"/>
+      <c r="H231" s="15"/>
+      <c r="I231" s="15"/>
+      <c r="J231" s="15"/>
+      <c r="K231" s="15"/>
+      <c r="L231" s="15"/>
+      <c r="M231" s="15"/>
+      <c r="N231" s="15"/>
+      <c r="O231" s="15"/>
+      <c r="P231" s="15"/>
+      <c r="Q231" s="15"/>
+      <c r="R231" s="15"/>
+      <c r="S231" s="15"/>
+      <c r="T231" s="9"/>
+      <c r="U231" s="15"/>
+    </row>
+    <row r="232" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A232" s="35"/>
+      <c r="B232" s="15"/>
+      <c r="C232" s="15"/>
+      <c r="D232" s="15"/>
+      <c r="E232" s="15"/>
+      <c r="F232" s="15"/>
+      <c r="G232" s="15"/>
+      <c r="H232" s="15"/>
+      <c r="I232" s="15"/>
+      <c r="J232" s="15"/>
+      <c r="K232" s="15"/>
+      <c r="L232" s="15"/>
+      <c r="M232" s="15"/>
+      <c r="N232" s="15"/>
+      <c r="O232" s="15"/>
+      <c r="P232" s="15"/>
+      <c r="Q232" s="15"/>
+      <c r="R232" s="15"/>
+      <c r="S232" s="15"/>
+      <c r="T232" s="9"/>
+      <c r="U232" s="15"/>
+    </row>
+    <row r="233" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A233" s="35"/>
+      <c r="B233" s="15"/>
+      <c r="C233" s="15"/>
+      <c r="D233" s="15"/>
+      <c r="E233" s="15"/>
+      <c r="F233" s="15"/>
+      <c r="G233" s="15"/>
+      <c r="H233" s="15"/>
+      <c r="I233" s="15"/>
+      <c r="J233" s="15"/>
+      <c r="K233" s="15"/>
+      <c r="L233" s="15"/>
+      <c r="M233" s="15"/>
+      <c r="N233" s="15"/>
+      <c r="O233" s="15"/>
+      <c r="P233" s="15"/>
+      <c r="Q233" s="15"/>
+      <c r="R233" s="15"/>
+      <c r="S233" s="15"/>
+      <c r="T233" s="9"/>
+      <c r="U233" s="15"/>
+    </row>
+    <row r="234" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A234" s="35"/>
+      <c r="B234" s="15"/>
+      <c r="C234" s="15"/>
+      <c r="D234" s="15"/>
+      <c r="E234" s="15"/>
+      <c r="F234" s="15"/>
+      <c r="G234" s="15"/>
+      <c r="H234" s="15"/>
+      <c r="I234" s="15"/>
+      <c r="J234" s="15"/>
+      <c r="K234" s="15"/>
+      <c r="L234" s="15"/>
+      <c r="M234" s="15"/>
+      <c r="N234" s="15"/>
+      <c r="O234" s="15"/>
+      <c r="P234" s="15"/>
+      <c r="Q234" s="15"/>
+      <c r="R234" s="15"/>
+      <c r="S234" s="15"/>
+      <c r="T234" s="9"/>
+      <c r="U234" s="15"/>
+    </row>
+    <row r="235" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A235" s="35"/>
+      <c r="B235" s="15"/>
+      <c r="C235" s="15"/>
+      <c r="D235" s="15"/>
+      <c r="E235" s="15"/>
+      <c r="F235" s="15"/>
+      <c r="G235" s="15"/>
+      <c r="H235" s="15"/>
+      <c r="I235" s="15"/>
+      <c r="J235" s="15"/>
+      <c r="K235" s="15"/>
+      <c r="L235" s="15"/>
+      <c r="M235" s="15"/>
+      <c r="N235" s="15"/>
+      <c r="O235" s="15"/>
+      <c r="P235" s="15"/>
+      <c r="Q235" s="15"/>
+      <c r="R235" s="15"/>
+      <c r="S235" s="15"/>
+      <c r="T235" s="9"/>
+      <c r="U235" s="15"/>
+    </row>
+    <row r="236" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A236" s="35"/>
+      <c r="B236" s="15"/>
+      <c r="C236" s="15"/>
+      <c r="D236" s="15"/>
+      <c r="E236" s="15"/>
+      <c r="F236" s="15"/>
+      <c r="G236" s="15"/>
+      <c r="H236" s="15"/>
+      <c r="I236" s="15"/>
+      <c r="J236" s="15"/>
+      <c r="K236" s="15"/>
+      <c r="L236" s="15"/>
+      <c r="M236" s="15"/>
+      <c r="N236" s="15"/>
+      <c r="O236" s="15"/>
+      <c r="P236" s="15"/>
+      <c r="Q236" s="15"/>
+      <c r="R236" s="15"/>
+      <c r="S236" s="15"/>
+      <c r="T236" s="9"/>
+      <c r="U236" s="15"/>
+    </row>
+    <row r="237" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A237" s="35"/>
+      <c r="B237" s="15"/>
+      <c r="C237" s="15"/>
+      <c r="D237" s="15"/>
+      <c r="E237" s="15"/>
+      <c r="F237" s="15"/>
+      <c r="G237" s="15"/>
+      <c r="H237" s="15"/>
+      <c r="I237" s="15"/>
+      <c r="J237" s="15"/>
+      <c r="K237" s="15"/>
+      <c r="L237" s="15"/>
+      <c r="M237" s="15"/>
+      <c r="N237" s="15"/>
+      <c r="O237" s="15"/>
+      <c r="P237" s="15"/>
+      <c r="Q237" s="15"/>
+      <c r="R237" s="15"/>
+      <c r="S237" s="15"/>
+      <c r="T237" s="9"/>
+      <c r="U237" s="15"/>
+    </row>
+    <row r="238" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A238" s="35"/>
+      <c r="B238" s="15"/>
+      <c r="C238" s="15"/>
+      <c r="D238" s="15"/>
+      <c r="E238" s="15"/>
+      <c r="F238" s="15"/>
+      <c r="G238" s="15"/>
+      <c r="H238" s="15"/>
+      <c r="I238" s="15"/>
+      <c r="J238" s="15"/>
+      <c r="K238" s="15"/>
+      <c r="L238" s="15"/>
+      <c r="M238" s="15"/>
+      <c r="N238" s="15"/>
+      <c r="O238" s="15"/>
+      <c r="P238" s="15"/>
+      <c r="Q238" s="15"/>
+      <c r="R238" s="15"/>
+      <c r="S238" s="15"/>
+      <c r="T238" s="9"/>
+      <c r="U238" s="15"/>
+    </row>
+    <row r="239" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A239" s="35"/>
+      <c r="B239" s="15"/>
+      <c r="C239" s="15"/>
+      <c r="D239" s="15"/>
+      <c r="E239" s="15"/>
+      <c r="F239" s="15"/>
+      <c r="G239" s="15"/>
+      <c r="H239" s="15"/>
+      <c r="I239" s="15"/>
+      <c r="J239" s="15"/>
+      <c r="K239" s="15"/>
+      <c r="L239" s="15"/>
+      <c r="M239" s="15"/>
+      <c r="N239" s="15"/>
+      <c r="O239" s="15"/>
+      <c r="P239" s="15"/>
+      <c r="Q239" s="15"/>
+      <c r="R239" s="15"/>
+      <c r="S239" s="15"/>
+      <c r="T239" s="9"/>
+      <c r="U239" s="15"/>
+    </row>
+    <row r="240" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A240" s="35"/>
+      <c r="B240" s="15"/>
+      <c r="C240" s="15"/>
+      <c r="D240" s="15"/>
+      <c r="E240" s="15"/>
+      <c r="F240" s="15"/>
+      <c r="G240" s="15"/>
+      <c r="H240" s="15"/>
+      <c r="I240" s="15"/>
+      <c r="J240" s="15"/>
+      <c r="K240" s="15"/>
+      <c r="L240" s="15"/>
+      <c r="M240" s="15"/>
+      <c r="N240" s="15"/>
+      <c r="O240" s="15"/>
+      <c r="P240" s="15"/>
+      <c r="Q240" s="15"/>
+      <c r="R240" s="15"/>
+      <c r="S240" s="15"/>
+      <c r="T240" s="9"/>
+      <c r="U240" s="15"/>
+    </row>
+    <row r="241" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A241" s="35"/>
+      <c r="B241" s="15"/>
+      <c r="C241" s="15"/>
+      <c r="D241" s="15"/>
+      <c r="E241" s="15"/>
+      <c r="F241" s="15"/>
+      <c r="G241" s="15"/>
+      <c r="H241" s="15"/>
+      <c r="I241" s="15"/>
+      <c r="J241" s="15"/>
+      <c r="K241" s="15"/>
+      <c r="L241" s="15"/>
+      <c r="M241" s="15"/>
+      <c r="N241" s="15"/>
+      <c r="O241" s="15"/>
+      <c r="P241" s="15"/>
+      <c r="Q241" s="15"/>
+      <c r="R241" s="15"/>
+      <c r="S241" s="15"/>
+      <c r="T241" s="9"/>
+      <c r="U241" s="15"/>
+    </row>
+    <row r="242" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A242" s="35"/>
+      <c r="B242" s="15"/>
+      <c r="C242" s="15"/>
+      <c r="D242" s="15"/>
+      <c r="E242" s="15"/>
+      <c r="F242" s="15"/>
+      <c r="G242" s="15"/>
+      <c r="H242" s="15"/>
+      <c r="I242" s="15"/>
+      <c r="J242" s="15"/>
+      <c r="K242" s="15"/>
+      <c r="L242" s="15"/>
+      <c r="M242" s="15"/>
+      <c r="N242" s="15"/>
+      <c r="O242" s="15"/>
+      <c r="P242" s="15"/>
+      <c r="Q242" s="15"/>
+      <c r="R242" s="15"/>
+      <c r="S242" s="15"/>
+      <c r="T242" s="9"/>
+      <c r="U242" s="15"/>
+    </row>
+    <row r="243" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A243" s="35"/>
+      <c r="B243" s="15"/>
+      <c r="C243" s="15"/>
+      <c r="D243" s="15"/>
+      <c r="E243" s="15"/>
+      <c r="F243" s="15"/>
+      <c r="G243" s="15"/>
+      <c r="H243" s="15"/>
+      <c r="I243" s="15"/>
+      <c r="J243" s="15"/>
+      <c r="K243" s="15"/>
+      <c r="L243" s="15"/>
+      <c r="M243" s="15"/>
+      <c r="N243" s="15"/>
+      <c r="O243" s="15"/>
+      <c r="P243" s="15"/>
+      <c r="Q243" s="15"/>
+      <c r="R243" s="15"/>
+      <c r="S243" s="15"/>
+      <c r="T243" s="9"/>
+      <c r="U243" s="15"/>
+    </row>
+    <row r="244" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A244" s="35"/>
+      <c r="B244" s="15"/>
+      <c r="C244" s="15"/>
+      <c r="D244" s="15"/>
+      <c r="E244" s="15"/>
+      <c r="F244" s="15"/>
+      <c r="G244" s="15"/>
+      <c r="H244" s="15"/>
+      <c r="I244" s="15"/>
+      <c r="J244" s="15"/>
+      <c r="K244" s="15"/>
+      <c r="L244" s="15"/>
+      <c r="M244" s="15"/>
+      <c r="N244" s="15"/>
+      <c r="O244" s="15"/>
+      <c r="P244" s="15"/>
+      <c r="Q244" s="15"/>
+      <c r="R244" s="15"/>
+      <c r="S244" s="15"/>
+      <c r="T244" s="9"/>
+      <c r="U244" s="15"/>
+    </row>
+    <row r="245" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A245" s="35"/>
+      <c r="B245" s="15"/>
+      <c r="C245" s="15"/>
+      <c r="D245" s="15"/>
+      <c r="E245" s="15"/>
+      <c r="F245" s="15"/>
+      <c r="G245" s="15"/>
+      <c r="H245" s="15"/>
+      <c r="I245" s="15"/>
+      <c r="J245" s="15"/>
+      <c r="K245" s="15"/>
+      <c r="L245" s="15"/>
+      <c r="M245" s="15"/>
+      <c r="N245" s="15"/>
+      <c r="O245" s="15"/>
+      <c r="P245" s="15"/>
+      <c r="Q245" s="15"/>
+      <c r="R245" s="15"/>
+      <c r="S245" s="15"/>
+      <c r="T245" s="9"/>
+      <c r="U245" s="15"/>
+    </row>
+    <row r="246" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A246" s="35"/>
+      <c r="B246" s="15"/>
+      <c r="C246" s="15"/>
+      <c r="D246" s="15"/>
+      <c r="E246" s="15"/>
+      <c r="F246" s="15"/>
+      <c r="G246" s="15"/>
+      <c r="H246" s="15"/>
+      <c r="I246" s="15"/>
+      <c r="J246" s="15"/>
+      <c r="K246" s="15"/>
+      <c r="L246" s="15"/>
+      <c r="M246" s="15"/>
+      <c r="N246" s="15"/>
+      <c r="O246" s="15"/>
+      <c r="P246" s="15"/>
+      <c r="Q246" s="15"/>
+      <c r="R246" s="15"/>
+      <c r="S246" s="15"/>
+      <c r="T246" s="9"/>
+      <c r="U246" s="15"/>
+    </row>
+    <row r="247" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A247" s="35"/>
+      <c r="B247" s="15"/>
+      <c r="C247" s="15"/>
+      <c r="D247" s="15"/>
+      <c r="E247" s="15"/>
+      <c r="F247" s="15"/>
+      <c r="G247" s="15"/>
+      <c r="H247" s="15"/>
+      <c r="I247" s="15"/>
+      <c r="J247" s="15"/>
+      <c r="K247" s="15"/>
+      <c r="L247" s="15"/>
+      <c r="M247" s="15"/>
+      <c r="N247" s="15"/>
+      <c r="O247" s="15"/>
+      <c r="P247" s="15"/>
+      <c r="Q247" s="15"/>
+      <c r="R247" s="15"/>
+      <c r="S247" s="15"/>
+      <c r="T247" s="9"/>
+      <c r="U247" s="15"/>
+    </row>
+    <row r="248" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A248" s="35"/>
+      <c r="B248" s="15"/>
+      <c r="C248" s="15"/>
+      <c r="D248" s="15"/>
+      <c r="E248" s="15"/>
+      <c r="F248" s="15"/>
+      <c r="G248" s="15"/>
+      <c r="H248" s="15"/>
+      <c r="I248" s="15"/>
+      <c r="J248" s="15"/>
+      <c r="K248" s="15"/>
+      <c r="L248" s="15"/>
+      <c r="M248" s="15"/>
+      <c r="N248" s="15"/>
+      <c r="O248" s="15"/>
+      <c r="P248" s="15"/>
+      <c r="Q248" s="15"/>
+      <c r="R248" s="15"/>
+      <c r="S248" s="15"/>
+      <c r="T248" s="9"/>
+      <c r="U248" s="15"/>
+    </row>
+    <row r="249" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A249" s="8"/>
+      <c r="B249" s="15"/>
+      <c r="C249" s="15"/>
+      <c r="D249" s="15"/>
+      <c r="E249" s="15"/>
+      <c r="F249" s="15"/>
+      <c r="G249" s="15"/>
+      <c r="H249" s="15"/>
+      <c r="I249" s="15"/>
+      <c r="J249" s="15"/>
+      <c r="K249" s="15"/>
+      <c r="L249" s="15"/>
+      <c r="M249" s="15"/>
+      <c r="N249" s="15"/>
+      <c r="O249" s="15"/>
+      <c r="P249" s="15"/>
+      <c r="Q249" s="15"/>
+      <c r="R249" s="15"/>
+      <c r="S249" s="15"/>
+      <c r="T249" s="9"/>
+      <c r="U249" s="15"/>
+    </row>
+    <row r="250" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A250" s="8"/>
+      <c r="B250" s="15"/>
+      <c r="C250" s="15"/>
+      <c r="D250" s="15"/>
+      <c r="E250" s="15"/>
+      <c r="F250" s="15"/>
+      <c r="G250" s="15"/>
+      <c r="H250" s="15"/>
+      <c r="I250" s="15"/>
+      <c r="J250" s="15"/>
+      <c r="K250" s="15"/>
+      <c r="L250" s="15"/>
+      <c r="M250" s="15"/>
+      <c r="N250" s="15"/>
+      <c r="O250" s="15"/>
+      <c r="P250" s="15"/>
+      <c r="Q250" s="15"/>
+      <c r="R250" s="15"/>
+      <c r="S250" s="15"/>
+      <c r="T250" s="9"/>
+      <c r="U250" s="15"/>
+    </row>
+    <row r="251" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A251" s="8"/>
+      <c r="B251" s="15"/>
+      <c r="C251" s="15"/>
+      <c r="D251" s="15"/>
+      <c r="E251" s="15"/>
+      <c r="F251" s="15"/>
+      <c r="G251" s="15"/>
+      <c r="H251" s="15"/>
+      <c r="I251" s="15"/>
+      <c r="J251" s="15"/>
+      <c r="K251" s="15"/>
+      <c r="L251" s="15"/>
+      <c r="M251" s="15"/>
+      <c r="N251" s="15"/>
+      <c r="O251" s="15"/>
+      <c r="P251" s="15"/>
+      <c r="Q251" s="15"/>
+      <c r="R251" s="15"/>
+      <c r="S251" s="15"/>
+      <c r="T251" s="9"/>
+      <c r="U251" s="15"/>
+    </row>
+    <row r="252" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A252" s="8"/>
+      <c r="B252" s="15"/>
+      <c r="C252" s="15"/>
+      <c r="D252" s="15"/>
+      <c r="E252" s="15"/>
+      <c r="F252" s="15"/>
+      <c r="G252" s="15"/>
+      <c r="H252" s="15"/>
+      <c r="I252" s="15"/>
+      <c r="J252" s="15"/>
+      <c r="K252" s="15"/>
+      <c r="L252" s="15"/>
+      <c r="M252" s="15"/>
+      <c r="N252" s="15"/>
+      <c r="O252" s="15"/>
+      <c r="P252" s="15"/>
+      <c r="Q252" s="15"/>
+      <c r="R252" s="15"/>
+      <c r="S252" s="15"/>
+      <c r="T252" s="9"/>
+      <c r="U252" s="15"/>
+    </row>
+    <row r="253" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A253" s="8"/>
+      <c r="B253" s="15"/>
+      <c r="C253" s="15"/>
+      <c r="D253" s="15"/>
+      <c r="E253" s="15"/>
+      <c r="F253" s="15"/>
+      <c r="G253" s="15"/>
+      <c r="H253" s="15"/>
+      <c r="I253" s="15"/>
+      <c r="J253" s="15"/>
+      <c r="K253" s="15"/>
+      <c r="L253" s="15"/>
+      <c r="M253" s="15"/>
+      <c r="N253" s="15"/>
+      <c r="O253" s="15"/>
+      <c r="P253" s="15"/>
+      <c r="Q253" s="15"/>
+      <c r="R253" s="15"/>
+      <c r="S253" s="15"/>
+      <c r="T253" s="9"/>
+      <c r="U253" s="15"/>
+    </row>
+    <row r="254" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A254" s="8"/>
+      <c r="B254" s="15"/>
+      <c r="C254" s="15"/>
+      <c r="D254" s="15"/>
+      <c r="E254" s="15"/>
+      <c r="F254" s="15"/>
+      <c r="G254" s="15"/>
+      <c r="H254" s="15"/>
+      <c r="I254" s="15"/>
+      <c r="J254" s="15"/>
+      <c r="K254" s="15"/>
+      <c r="L254" s="15"/>
+      <c r="M254" s="15"/>
+      <c r="N254" s="15"/>
+      <c r="O254" s="15"/>
+      <c r="P254" s="15"/>
+      <c r="Q254" s="15"/>
+      <c r="R254" s="15"/>
+      <c r="S254" s="15"/>
+      <c r="T254" s="9"/>
+      <c r="U254" s="15"/>
+    </row>
+    <row r="255" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A255" s="8"/>
+      <c r="B255" s="15"/>
+      <c r="C255" s="15"/>
+      <c r="D255" s="15"/>
+      <c r="E255" s="15"/>
+      <c r="F255" s="15"/>
+      <c r="G255" s="15"/>
+      <c r="H255" s="15"/>
+      <c r="I255" s="15"/>
+      <c r="J255" s="15"/>
+      <c r="K255" s="15"/>
+      <c r="L255" s="15"/>
+      <c r="M255" s="15"/>
+      <c r="N255" s="15"/>
+      <c r="O255" s="15"/>
+      <c r="P255" s="15"/>
+      <c r="Q255" s="15"/>
+      <c r="R255" s="15"/>
+      <c r="S255" s="15"/>
+      <c r="T255" s="9"/>
+      <c r="U255" s="15"/>
+    </row>
+    <row r="256" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A256" s="8"/>
+      <c r="B256" s="15"/>
+      <c r="C256" s="15"/>
+      <c r="D256" s="15"/>
+      <c r="E256" s="15"/>
+      <c r="F256" s="15"/>
+      <c r="G256" s="15"/>
+      <c r="H256" s="15"/>
+      <c r="I256" s="15"/>
+      <c r="J256" s="15"/>
+      <c r="K256" s="15"/>
+      <c r="L256" s="15"/>
+      <c r="M256" s="15"/>
+      <c r="N256" s="15"/>
+      <c r="O256" s="15"/>
+      <c r="P256" s="15"/>
+      <c r="Q256" s="15"/>
+      <c r="R256" s="15"/>
+      <c r="S256" s="15"/>
+      <c r="T256" s="9"/>
+      <c r="U256" s="15"/>
+    </row>
+    <row r="257" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A257" s="8"/>
+      <c r="B257" s="15"/>
+      <c r="C257" s="15"/>
+      <c r="D257" s="15"/>
+      <c r="E257" s="15"/>
+      <c r="F257" s="15"/>
+      <c r="G257" s="15"/>
+      <c r="H257" s="15"/>
+      <c r="I257" s="15"/>
+      <c r="J257" s="15"/>
+      <c r="K257" s="15"/>
+      <c r="L257" s="15"/>
+      <c r="M257" s="15"/>
+      <c r="N257" s="15"/>
+      <c r="O257" s="15"/>
+      <c r="P257" s="15"/>
+      <c r="Q257" s="15"/>
+      <c r="R257" s="15"/>
+      <c r="S257" s="15"/>
+      <c r="T257" s="9"/>
+      <c r="U257" s="15"/>
+    </row>
+    <row r="258" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A258" s="8"/>
+      <c r="B258" s="15"/>
+      <c r="C258" s="15"/>
+      <c r="D258" s="15"/>
+      <c r="E258" s="15"/>
+      <c r="F258" s="15"/>
+      <c r="G258" s="15"/>
+      <c r="H258" s="15"/>
+      <c r="I258" s="15"/>
+      <c r="J258" s="15"/>
+      <c r="K258" s="15"/>
+      <c r="L258" s="15"/>
+      <c r="M258" s="15"/>
+      <c r="N258" s="15"/>
+      <c r="O258" s="15"/>
+      <c r="P258" s="15"/>
+      <c r="Q258" s="15"/>
+      <c r="R258" s="15"/>
+      <c r="S258" s="15"/>
+      <c r="T258" s="9"/>
+      <c r="U258" s="15"/>
+    </row>
+    <row r="259" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A259" s="8"/>
+      <c r="B259" s="15"/>
+      <c r="C259" s="15"/>
+      <c r="D259" s="15"/>
+      <c r="E259" s="15"/>
+      <c r="F259" s="15"/>
+      <c r="G259" s="15"/>
+      <c r="H259" s="15"/>
+      <c r="I259" s="15"/>
+      <c r="J259" s="15"/>
+      <c r="K259" s="15"/>
+      <c r="L259" s="15"/>
+      <c r="M259" s="15"/>
+      <c r="N259" s="15"/>
+      <c r="O259" s="15"/>
+      <c r="P259" s="15"/>
+      <c r="Q259" s="15"/>
+      <c r="R259" s="15"/>
+      <c r="S259" s="15"/>
+      <c r="T259" s="9"/>
+      <c r="U259" s="15"/>
+    </row>
+    <row r="260" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A260" s="10"/>
+      <c r="B260" s="11"/>
+      <c r="C260" s="11"/>
+      <c r="D260" s="11"/>
+      <c r="E260" s="11"/>
+      <c r="F260" s="11"/>
+      <c r="G260" s="11"/>
+      <c r="H260" s="11"/>
+      <c r="I260" s="11"/>
+      <c r="J260" s="11"/>
+      <c r="K260" s="11"/>
+      <c r="L260" s="11"/>
+      <c r="M260" s="11"/>
+      <c r="N260" s="11"/>
+      <c r="O260" s="11"/>
+      <c r="P260" s="11"/>
+      <c r="Q260" s="11"/>
+      <c r="R260" s="11"/>
+      <c r="S260" s="11"/>
+      <c r="T260" s="13"/>
+      <c r="U260" s="15"/>
+    </row>
+    <row r="263" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A263" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B263" s="6"/>
+      <c r="C263" s="6"/>
+      <c r="D263" s="6"/>
+      <c r="E263" s="6"/>
+      <c r="F263" s="6"/>
+      <c r="G263" s="6"/>
+      <c r="H263" s="6"/>
+      <c r="I263" s="6"/>
+      <c r="J263" s="6"/>
+      <c r="K263" s="6"/>
+      <c r="L263" s="6"/>
+      <c r="M263" s="6"/>
+      <c r="N263" s="6"/>
+      <c r="O263" s="6"/>
+      <c r="P263" s="6"/>
+      <c r="Q263" s="6"/>
+      <c r="R263" s="7"/>
+    </row>
+    <row r="264" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A264" s="8"/>
+      <c r="B264" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C264" s="15"/>
+      <c r="D264" s="15"/>
+      <c r="E264" s="15"/>
+      <c r="F264" s="15"/>
+      <c r="G264" s="15"/>
+      <c r="H264" s="15"/>
+      <c r="I264" s="15"/>
+      <c r="J264" s="15"/>
+      <c r="K264" s="15"/>
+      <c r="L264" s="15"/>
+      <c r="M264" s="15"/>
+      <c r="N264" s="15"/>
+      <c r="O264" s="15"/>
+      <c r="P264" s="15"/>
+      <c r="Q264" s="15"/>
+      <c r="R264" s="9"/>
+    </row>
+    <row r="265" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A265" s="8"/>
+      <c r="B265" s="15"/>
+      <c r="C265" s="15"/>
+      <c r="D265" s="15"/>
+      <c r="E265" s="15"/>
+      <c r="F265" s="15"/>
+      <c r="G265" s="15"/>
+      <c r="H265" s="15"/>
+      <c r="I265" s="15"/>
+      <c r="J265" s="15"/>
+      <c r="K265" s="15"/>
+      <c r="L265" s="15"/>
+      <c r="M265" s="15"/>
+      <c r="N265" s="15"/>
+      <c r="O265" s="15"/>
+      <c r="P265" s="15"/>
+      <c r="Q265" s="15"/>
+      <c r="R265" s="9"/>
+    </row>
+    <row r="266" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A266" s="8"/>
+      <c r="B266" s="15"/>
+      <c r="C266" s="15"/>
+      <c r="D266" s="15"/>
+      <c r="E266" s="15"/>
+      <c r="F266" s="15"/>
+      <c r="G266" s="15"/>
+      <c r="H266" s="15"/>
+      <c r="I266" s="15"/>
+      <c r="J266" s="15"/>
+      <c r="K266" s="15"/>
+      <c r="L266" s="15"/>
+      <c r="M266" s="15"/>
+      <c r="N266" s="15"/>
+      <c r="O266" s="15"/>
+      <c r="P266" s="15"/>
+      <c r="Q266" s="15"/>
+      <c r="R266" s="9"/>
+    </row>
+    <row r="267" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A267" s="8"/>
+      <c r="B267" s="15"/>
+      <c r="C267" s="15"/>
+      <c r="D267" s="15"/>
+      <c r="E267" s="15"/>
+      <c r="F267" s="15"/>
+      <c r="G267" s="15"/>
+      <c r="H267" s="15"/>
+      <c r="I267" s="15"/>
+      <c r="J267" s="15"/>
+      <c r="K267" s="15"/>
+      <c r="L267" s="15"/>
+      <c r="M267" s="15"/>
+      <c r="N267" s="15"/>
+      <c r="O267" s="15"/>
+      <c r="P267" s="15"/>
+      <c r="Q267" s="15"/>
+      <c r="R267" s="9"/>
+    </row>
+    <row r="268" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A268" s="8"/>
+      <c r="B268" s="15"/>
+      <c r="C268" s="15"/>
+      <c r="D268" s="15"/>
+      <c r="E268" s="15"/>
+      <c r="F268" s="15"/>
+      <c r="G268" s="15"/>
+      <c r="H268" s="15"/>
+      <c r="I268" s="15"/>
+      <c r="J268" s="15"/>
+      <c r="K268" s="15"/>
+      <c r="L268" s="15"/>
+      <c r="M268" s="15"/>
+      <c r="N268" s="15"/>
+      <c r="O268" s="15"/>
+      <c r="P268" s="15"/>
+      <c r="Q268" s="15"/>
+      <c r="R268" s="9"/>
+    </row>
+    <row r="269" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A269" s="8"/>
+      <c r="B269" s="15"/>
+      <c r="C269" s="15"/>
+      <c r="D269" s="15"/>
+      <c r="E269" s="15"/>
+      <c r="F269" s="15"/>
+      <c r="G269" s="15"/>
+      <c r="H269" s="15"/>
+      <c r="I269" s="15"/>
+      <c r="J269" s="15"/>
+      <c r="K269" s="15"/>
+      <c r="L269" s="15"/>
+      <c r="M269" s="15"/>
+      <c r="N269" s="15"/>
+      <c r="O269" s="15"/>
+      <c r="P269" s="15"/>
+      <c r="Q269" s="15"/>
+      <c r="R269" s="9"/>
+    </row>
+    <row r="270" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A270" s="8"/>
+      <c r="B270" s="15"/>
+      <c r="C270" s="15"/>
+      <c r="D270" s="15"/>
+      <c r="E270" s="15"/>
+      <c r="F270" s="15"/>
+      <c r="G270" s="15"/>
+      <c r="H270" s="15"/>
+      <c r="I270" s="15"/>
+      <c r="J270" s="15"/>
+      <c r="K270" s="15"/>
+      <c r="L270" s="15"/>
+      <c r="M270" s="15"/>
+      <c r="N270" s="15"/>
+      <c r="O270" s="15"/>
+      <c r="P270" s="15"/>
+      <c r="Q270" s="15"/>
+      <c r="R270" s="9"/>
+    </row>
+    <row r="271" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A271" s="8"/>
+      <c r="B271" s="15"/>
+      <c r="C271" s="15"/>
+      <c r="D271" s="15"/>
+      <c r="E271" s="15"/>
+      <c r="F271" s="15"/>
+      <c r="G271" s="15"/>
+      <c r="H271" s="15"/>
+      <c r="I271" s="15"/>
+      <c r="J271" s="15"/>
+      <c r="K271" s="15"/>
+      <c r="L271" s="15"/>
+      <c r="M271" s="15"/>
+      <c r="N271" s="15"/>
+      <c r="O271" s="15"/>
+      <c r="P271" s="15"/>
+      <c r="Q271" s="15"/>
+      <c r="R271" s="9"/>
+    </row>
+    <row r="272" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A272" s="8"/>
+      <c r="B272" s="15"/>
+      <c r="C272" s="15"/>
+      <c r="D272" s="15"/>
+      <c r="E272" s="15"/>
+      <c r="F272" s="15"/>
+      <c r="G272" s="15"/>
+      <c r="H272" s="15"/>
+      <c r="I272" s="15"/>
+      <c r="J272" s="15"/>
+      <c r="K272" s="15"/>
+      <c r="L272" s="15"/>
+      <c r="M272" s="15"/>
+      <c r="N272" s="15"/>
+      <c r="O272" s="15"/>
+      <c r="P272" s="15"/>
+      <c r="Q272" s="15"/>
+      <c r="R272" s="9"/>
+    </row>
+    <row r="273" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A273" s="8"/>
+      <c r="B273" s="15"/>
+      <c r="C273" s="15"/>
+      <c r="D273" s="15"/>
+      <c r="E273" s="15"/>
+      <c r="F273" s="15"/>
+      <c r="G273" s="15"/>
+      <c r="H273" s="15"/>
+      <c r="I273" s="15"/>
+      <c r="J273" s="15"/>
+      <c r="K273" s="15"/>
+      <c r="L273" s="15"/>
+      <c r="M273" s="15"/>
+      <c r="N273" s="15"/>
+      <c r="O273" s="15"/>
+      <c r="P273" s="15"/>
+      <c r="Q273" s="15"/>
+      <c r="R273" s="9"/>
+    </row>
+    <row r="274" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A274" s="8"/>
+      <c r="B274" s="15"/>
+      <c r="C274" s="15"/>
+      <c r="D274" s="15"/>
+      <c r="E274" s="29"/>
+      <c r="F274" s="15"/>
+      <c r="G274" s="15"/>
+      <c r="H274" s="15"/>
+      <c r="I274" s="15"/>
+      <c r="J274" s="15"/>
+      <c r="K274" s="15"/>
+      <c r="L274" s="15"/>
+      <c r="M274" s="15"/>
+      <c r="N274" s="15"/>
+      <c r="O274" s="15"/>
+      <c r="P274" s="15"/>
+      <c r="Q274" s="15"/>
+      <c r="R274" s="9"/>
+    </row>
+    <row r="275" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A275" s="8"/>
+      <c r="B275" s="15"/>
+      <c r="C275" s="15"/>
+      <c r="D275" s="15"/>
+      <c r="E275" s="15"/>
+      <c r="F275" s="15"/>
+      <c r="G275" s="15"/>
+      <c r="H275" s="15"/>
+      <c r="I275" s="15"/>
+      <c r="J275" s="15"/>
+      <c r="K275" s="15"/>
+      <c r="L275" s="15"/>
+      <c r="M275" s="15"/>
+      <c r="N275" s="15"/>
+      <c r="O275" s="15"/>
+      <c r="P275" s="15"/>
+      <c r="Q275" s="15"/>
+      <c r="R275" s="9"/>
+    </row>
+    <row r="276" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A276" s="8"/>
+      <c r="B276" s="15"/>
+      <c r="C276" s="15"/>
+      <c r="D276" s="15"/>
+      <c r="E276" s="15"/>
+      <c r="F276" s="15"/>
+      <c r="G276" s="15"/>
+      <c r="H276" s="15"/>
+      <c r="I276" s="15"/>
+      <c r="J276" s="15"/>
+      <c r="K276" s="15"/>
+      <c r="L276" s="15"/>
+      <c r="M276" s="15"/>
+      <c r="N276" s="15"/>
+      <c r="O276" s="15"/>
+      <c r="P276" s="15"/>
+      <c r="Q276" s="15"/>
+      <c r="R276" s="9"/>
+    </row>
+    <row r="277" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A277" s="8"/>
+      <c r="B277" s="15"/>
+      <c r="C277" s="15"/>
+      <c r="D277" s="15"/>
+      <c r="E277" s="15"/>
+      <c r="F277" s="15"/>
+      <c r="G277" s="15"/>
+      <c r="H277" s="15"/>
+      <c r="I277" s="15"/>
+      <c r="J277" s="15"/>
+      <c r="K277" s="15"/>
+      <c r="L277" s="15"/>
+      <c r="M277" s="15"/>
+      <c r="N277" s="15"/>
+      <c r="O277" s="15"/>
+      <c r="P277" s="15"/>
+      <c r="Q277" s="15"/>
+      <c r="R277" s="9"/>
+    </row>
+    <row r="278" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A278" s="8"/>
+      <c r="B278" s="15"/>
+      <c r="C278" s="15"/>
+      <c r="D278" s="15"/>
+      <c r="E278" s="15"/>
+      <c r="F278" s="15"/>
+      <c r="G278" s="15"/>
+      <c r="H278" s="15"/>
+      <c r="I278" s="15"/>
+      <c r="J278" s="15"/>
+      <c r="K278" s="15"/>
+      <c r="L278" s="15"/>
+      <c r="M278" s="15"/>
+      <c r="N278" s="15"/>
+      <c r="O278" s="15"/>
+      <c r="P278" s="15"/>
+      <c r="Q278" s="15"/>
+      <c r="R278" s="9"/>
+    </row>
+    <row r="279" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A279" s="8"/>
+      <c r="B279" s="15"/>
+      <c r="C279" s="15"/>
+      <c r="D279" s="15"/>
+      <c r="E279" s="15"/>
+      <c r="F279" s="15"/>
+      <c r="G279" s="15"/>
+      <c r="H279" s="15"/>
+      <c r="I279" s="15"/>
+      <c r="J279" s="15"/>
+      <c r="K279" s="15"/>
+      <c r="L279" s="15"/>
+      <c r="M279" s="15"/>
+      <c r="N279" s="15"/>
+      <c r="O279" s="15"/>
+      <c r="P279" s="15"/>
+      <c r="Q279" s="15"/>
+      <c r="R279" s="9"/>
+    </row>
+    <row r="280" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A280" s="8"/>
+      <c r="B280" s="15"/>
+      <c r="C280" s="15"/>
+      <c r="D280" s="15"/>
+      <c r="E280" s="15"/>
+      <c r="F280" s="15"/>
+      <c r="G280" s="15"/>
+      <c r="H280" s="15"/>
+      <c r="I280" s="15"/>
+      <c r="J280" s="15"/>
+      <c r="K280" s="15"/>
+      <c r="L280" s="15"/>
+      <c r="M280" s="15"/>
+      <c r="N280" s="15"/>
+      <c r="O280" s="15"/>
+      <c r="P280" s="15"/>
+      <c r="Q280" s="15"/>
+      <c r="R280" s="9"/>
+    </row>
+    <row r="281" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A281" s="8"/>
+      <c r="B281" s="15"/>
+      <c r="C281" s="15"/>
+      <c r="D281" s="15"/>
+      <c r="E281" s="15"/>
+      <c r="F281" s="15"/>
+      <c r="G281" s="15"/>
+      <c r="H281" s="15"/>
+      <c r="I281" s="15"/>
+      <c r="J281" s="15"/>
+      <c r="K281" s="15"/>
+      <c r="L281" s="15"/>
+      <c r="M281" s="15"/>
+      <c r="N281" s="15"/>
+      <c r="O281" s="15"/>
+      <c r="P281" s="15"/>
+      <c r="Q281" s="15"/>
+      <c r="R281" s="9"/>
+    </row>
+    <row r="282" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A282" s="8"/>
+      <c r="B282" s="15"/>
+      <c r="C282" s="15"/>
+      <c r="D282" s="15"/>
+      <c r="E282" s="15"/>
+      <c r="F282" s="15"/>
+      <c r="G282" s="15"/>
+      <c r="H282" s="15"/>
+      <c r="I282" s="15"/>
+      <c r="J282" s="15"/>
+      <c r="K282" s="15"/>
+      <c r="L282" s="15"/>
+      <c r="M282" s="15"/>
+      <c r="N282" s="15"/>
+      <c r="O282" s="15"/>
+      <c r="P282" s="15"/>
+      <c r="Q282" s="15"/>
+      <c r="R282" s="9"/>
+    </row>
+    <row r="283" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A283" s="8"/>
+      <c r="B283" s="15"/>
+      <c r="C283" s="15"/>
+      <c r="D283" s="15"/>
+      <c r="E283" s="15"/>
+      <c r="F283" s="15"/>
+      <c r="G283" s="15"/>
+      <c r="H283" s="15"/>
+      <c r="I283" s="15"/>
+      <c r="J283" s="15"/>
+      <c r="K283" s="15"/>
+      <c r="L283" s="15"/>
+      <c r="M283" s="15"/>
+      <c r="N283" s="15"/>
+      <c r="O283" s="15"/>
+      <c r="P283" s="15"/>
+      <c r="Q283" s="15"/>
+      <c r="R283" s="9"/>
+    </row>
+    <row r="284" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A284" s="8"/>
+      <c r="B284" s="15"/>
+      <c r="C284" s="15"/>
+      <c r="D284" s="15"/>
+      <c r="E284" s="15"/>
+      <c r="F284" s="15"/>
+      <c r="G284" s="15"/>
+      <c r="H284" s="15"/>
+      <c r="I284" s="15"/>
+      <c r="J284" s="15"/>
+      <c r="K284" s="15"/>
+      <c r="L284" s="15"/>
+      <c r="M284" s="15"/>
+      <c r="N284" s="15"/>
+      <c r="O284" s="15"/>
+      <c r="P284" s="15"/>
+      <c r="Q284" s="15"/>
+      <c r="R284" s="9"/>
+    </row>
+    <row r="285" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A285" s="8"/>
+      <c r="B285" s="15"/>
+      <c r="C285" s="15"/>
+      <c r="D285" s="15"/>
+      <c r="E285" s="15"/>
+      <c r="F285" s="15"/>
+      <c r="G285" s="15"/>
+      <c r="H285" s="15"/>
+      <c r="I285" s="15"/>
+      <c r="J285" s="15"/>
+      <c r="K285" s="15"/>
+      <c r="L285" s="15"/>
+      <c r="M285" s="15"/>
+      <c r="N285" s="15"/>
+      <c r="O285" s="15"/>
+      <c r="P285" s="15"/>
+      <c r="Q285" s="15"/>
+      <c r="R285" s="9"/>
+    </row>
+    <row r="286" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A286" s="8"/>
+      <c r="B286" s="15"/>
+      <c r="C286" s="15"/>
+      <c r="D286" s="15"/>
+      <c r="E286" s="15"/>
+      <c r="F286" s="15"/>
+      <c r="G286" s="15"/>
+      <c r="H286" s="15"/>
+      <c r="I286" s="15"/>
+      <c r="J286" s="15"/>
+      <c r="K286" s="15"/>
+      <c r="L286" s="15"/>
+      <c r="M286" s="15"/>
+      <c r="N286" s="15"/>
+      <c r="O286" s="15"/>
+      <c r="P286" s="15"/>
+      <c r="Q286" s="15"/>
+      <c r="R286" s="9"/>
+    </row>
+    <row r="287" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A287" s="8"/>
+      <c r="B287" s="15"/>
+      <c r="C287" s="15"/>
+      <c r="D287" s="15"/>
+      <c r="E287" s="15"/>
+      <c r="F287" s="15"/>
+      <c r="G287" s="15"/>
+      <c r="H287" s="15"/>
+      <c r="I287" s="15"/>
+      <c r="J287" s="15"/>
+      <c r="K287" s="15"/>
+      <c r="L287" s="15"/>
+      <c r="M287" s="15"/>
+      <c r="N287" s="15"/>
+      <c r="O287" s="15"/>
+      <c r="P287" s="15"/>
+      <c r="Q287" s="15"/>
+      <c r="R287" s="9"/>
+    </row>
+    <row r="288" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A288" s="8"/>
+      <c r="B288" s="15"/>
+      <c r="C288" s="15"/>
+      <c r="D288" s="15"/>
+      <c r="E288" s="15"/>
+      <c r="F288" s="15"/>
+      <c r="G288" s="15"/>
+      <c r="H288" s="15"/>
+      <c r="I288" s="15"/>
+      <c r="J288" s="15"/>
+      <c r="K288" s="15"/>
+      <c r="L288" s="15"/>
+      <c r="M288" s="15"/>
+      <c r="N288" s="15"/>
+      <c r="O288" s="15"/>
+      <c r="P288" s="15"/>
+      <c r="Q288" s="15"/>
+      <c r="R288" s="9"/>
+    </row>
+    <row r="289" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A289" s="8"/>
+      <c r="B289" s="15"/>
+      <c r="C289" s="15"/>
+      <c r="D289" s="15"/>
+      <c r="E289" s="15"/>
+      <c r="F289" s="15"/>
+      <c r="G289" s="15"/>
+      <c r="H289" s="15"/>
+      <c r="I289" s="15"/>
+      <c r="J289" s="15"/>
+      <c r="K289" s="15"/>
+      <c r="L289" s="15"/>
+      <c r="M289" s="15"/>
+      <c r="N289" s="15"/>
+      <c r="O289" s="15"/>
+      <c r="P289" s="15"/>
+      <c r="Q289" s="15"/>
+      <c r="R289" s="9"/>
+    </row>
+    <row r="290" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A290" s="8"/>
+      <c r="B290" s="15"/>
+      <c r="C290" s="15"/>
+      <c r="D290" s="15"/>
+      <c r="E290" s="15"/>
+      <c r="F290" s="15"/>
+      <c r="G290" s="15"/>
+      <c r="H290" s="15"/>
+      <c r="I290" s="15"/>
+      <c r="J290" s="15"/>
+      <c r="K290" s="15"/>
+      <c r="L290" s="15"/>
+      <c r="M290" s="15"/>
+      <c r="N290" s="15"/>
+      <c r="O290" s="15"/>
+      <c r="P290" s="15"/>
+      <c r="Q290" s="15"/>
+      <c r="R290" s="9"/>
+    </row>
+    <row r="291" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A291" s="8"/>
+      <c r="B291" s="15"/>
+      <c r="C291" s="15"/>
+      <c r="D291" s="15"/>
+      <c r="E291" s="15"/>
+      <c r="F291" s="15"/>
+      <c r="G291" s="15"/>
+      <c r="H291" s="15"/>
+      <c r="I291" s="15"/>
+      <c r="J291" s="15"/>
+      <c r="K291" s="15"/>
+      <c r="L291" s="15"/>
+      <c r="M291" s="15"/>
+      <c r="N291" s="15"/>
+      <c r="O291" s="15"/>
+      <c r="P291" s="15"/>
+      <c r="Q291" s="15"/>
+      <c r="R291" s="9"/>
+    </row>
+    <row r="292" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A292" s="8"/>
+      <c r="B292" s="15"/>
+      <c r="C292" s="15"/>
+      <c r="D292" s="15"/>
+      <c r="E292" s="15"/>
+      <c r="F292" s="15"/>
+      <c r="G292" s="15"/>
+      <c r="H292" s="15"/>
+      <c r="I292" s="15"/>
+      <c r="J292" s="15"/>
+      <c r="K292" s="15"/>
+      <c r="L292" s="15"/>
+      <c r="M292" s="15"/>
+      <c r="N292" s="15"/>
+      <c r="O292" s="15"/>
+      <c r="P292" s="15"/>
+      <c r="Q292" s="15"/>
+      <c r="R292" s="9"/>
+    </row>
+    <row r="293" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A293" s="8"/>
+      <c r="B293" s="15"/>
+      <c r="C293" s="15"/>
+      <c r="D293" s="15"/>
+      <c r="E293" s="15"/>
+      <c r="F293" s="15"/>
+      <c r="G293" s="15"/>
+      <c r="H293" s="15"/>
+      <c r="I293" s="15"/>
+      <c r="J293" s="15"/>
+      <c r="K293" s="15"/>
+      <c r="L293" s="15"/>
+      <c r="M293" s="15"/>
+      <c r="N293" s="15"/>
+      <c r="O293" s="15"/>
+      <c r="P293" s="15"/>
+      <c r="Q293" s="15"/>
+      <c r="R293" s="9"/>
+    </row>
+    <row r="294" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A294" s="8"/>
+      <c r="B294" s="15"/>
+      <c r="C294" s="15"/>
+      <c r="D294" s="15"/>
+      <c r="E294" s="15"/>
+      <c r="F294" s="15"/>
+      <c r="G294" s="15"/>
+      <c r="H294" s="15"/>
+      <c r="I294" s="15"/>
+      <c r="J294" s="15"/>
+      <c r="K294" s="15"/>
+      <c r="L294" s="15"/>
+      <c r="M294" s="15"/>
+      <c r="N294" s="15"/>
+      <c r="O294" s="15"/>
+      <c r="P294" s="15"/>
+      <c r="Q294" s="15"/>
+      <c r="R294" s="9"/>
+    </row>
+    <row r="295" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A295" s="10"/>
+      <c r="B295" s="11"/>
+      <c r="C295" s="11"/>
+      <c r="D295" s="11"/>
+      <c r="E295" s="11"/>
+      <c r="F295" s="11"/>
+      <c r="G295" s="11"/>
+      <c r="H295" s="11"/>
+      <c r="I295" s="11"/>
+      <c r="J295" s="11"/>
+      <c r="K295" s="11"/>
+      <c r="L295" s="11"/>
+      <c r="M295" s="11"/>
+      <c r="N295" s="11"/>
+      <c r="O295" s="11"/>
+      <c r="P295" s="11"/>
+      <c r="Q295" s="11"/>
+      <c r="R295" s="13"/>
+    </row>
+    <row r="298" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="299" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B299" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C299" s="6"/>
+      <c r="D299" s="6"/>
+      <c r="E299" s="6"/>
+      <c r="F299" s="6"/>
+      <c r="G299" s="6"/>
+      <c r="H299" s="6"/>
+      <c r="I299" s="6"/>
+      <c r="J299" s="7"/>
+    </row>
+    <row r="300" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B300" s="8"/>
+      <c r="C300" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D300" s="15"/>
+      <c r="E300" s="15"/>
+      <c r="F300" s="15"/>
+      <c r="G300" s="15"/>
+      <c r="H300" s="15"/>
+      <c r="I300" s="15"/>
+      <c r="J300" s="9"/>
+    </row>
+    <row r="301" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B301" s="8"/>
+      <c r="C301" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D301" s="29"/>
+      <c r="E301" s="15"/>
+      <c r="F301" s="15"/>
+      <c r="G301" s="15"/>
+      <c r="H301" s="15"/>
+      <c r="I301" s="15"/>
+      <c r="J301" s="9"/>
+    </row>
+    <row r="302" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B302" s="8"/>
+      <c r="C302" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D302" s="30"/>
+      <c r="E302" s="30"/>
+      <c r="F302" s="30"/>
+      <c r="G302" s="15"/>
+      <c r="H302" s="15"/>
+      <c r="I302" s="15"/>
+      <c r="J302" s="9"/>
+    </row>
+    <row r="303" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B303" s="8"/>
+      <c r="C303" s="30"/>
+      <c r="D303" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E303" s="30"/>
+      <c r="F303" s="30"/>
+      <c r="G303" s="15"/>
+      <c r="H303" s="15"/>
+      <c r="I303" s="15"/>
+      <c r="J303" s="9"/>
+    </row>
+    <row r="304" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B304" s="8"/>
+      <c r="C304" s="30"/>
+      <c r="D304" s="30"/>
+      <c r="E304" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F304" s="30"/>
+      <c r="G304" s="15"/>
+      <c r="H304" s="15"/>
+      <c r="I304" s="15"/>
+      <c r="J304" s="9"/>
+    </row>
+    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B305" s="8"/>
+      <c r="C305" s="30"/>
+      <c r="D305" s="30"/>
+      <c r="E305" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F305" s="30"/>
+      <c r="G305" s="15"/>
+      <c r="H305" s="15"/>
+      <c r="I305" s="15"/>
+      <c r="J305" s="9"/>
+    </row>
+    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B306" s="8"/>
+      <c r="C306" s="15"/>
+      <c r="D306" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E306" s="29"/>
+      <c r="F306" s="15"/>
+      <c r="G306" s="15"/>
+      <c r="H306" s="15"/>
+      <c r="I306" s="15"/>
+      <c r="J306" s="9"/>
+      <c r="K306" t="s">
+        <v>26</v>
+      </c>
+      <c r="L306" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B307" s="8"/>
+      <c r="C307" s="15"/>
+      <c r="D307" s="29"/>
+      <c r="E307" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F307" s="7"/>
+      <c r="G307" s="15"/>
+      <c r="H307" s="15"/>
+      <c r="I307" s="15"/>
+      <c r="J307" s="9"/>
+      <c r="K307" t="s">
+        <v>26</v>
+      </c>
+      <c r="L307" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B308" s="8"/>
+      <c r="C308" s="15"/>
+      <c r="D308" s="29"/>
+      <c r="E308" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="F308" s="9"/>
+      <c r="G308" s="15"/>
+      <c r="H308" s="15"/>
+      <c r="I308" s="15"/>
+      <c r="J308" s="9"/>
+      <c r="K308" t="s">
+        <v>26</v>
+      </c>
+      <c r="L308" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B309" s="8"/>
+      <c r="C309" s="15"/>
+      <c r="D309" s="29"/>
+      <c r="E309" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="F309" s="13"/>
+      <c r="G309" s="15"/>
+      <c r="H309" s="15"/>
+      <c r="I309" s="15"/>
+      <c r="J309" s="9"/>
+      <c r="K309" t="s">
+        <v>26</v>
+      </c>
+      <c r="L309" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B310" s="10"/>
+      <c r="C310" s="11"/>
+      <c r="D310" s="11"/>
+      <c r="E310" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F310" s="11"/>
+      <c r="G310" s="11"/>
+      <c r="H310" s="11"/>
+      <c r="I310" s="11"/>
+      <c r="J310" s="13"/>
+      <c r="K310" t="s">
+        <v>26</v>
+      </c>
+      <c r="L310" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="313" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B314" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C314" s="6"/>
+      <c r="D314" s="6"/>
+      <c r="E314" s="6"/>
+      <c r="F314" s="6"/>
+      <c r="G314" s="6"/>
+      <c r="H314" s="6"/>
+      <c r="I314" s="7"/>
+    </row>
+    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B315" s="8"/>
+      <c r="C315" s="15"/>
+      <c r="D315" s="15"/>
+      <c r="E315" s="15"/>
+      <c r="F315" s="15"/>
+      <c r="G315" s="15"/>
+      <c r="H315" s="15"/>
+      <c r="I315" s="9"/>
+    </row>
+    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B316" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C316" s="15"/>
+      <c r="D316" s="15"/>
+      <c r="E316" s="15"/>
+      <c r="F316" s="15"/>
+      <c r="G316" s="15"/>
+      <c r="H316" s="15"/>
+      <c r="I316" s="9"/>
+    </row>
+    <row r="317" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B317" s="8"/>
+      <c r="C317" s="15"/>
+      <c r="D317" s="15"/>
+      <c r="E317" s="15"/>
+      <c r="F317" s="15"/>
+      <c r="G317" s="15"/>
+      <c r="H317" s="15"/>
+      <c r="I317" s="9"/>
+    </row>
+    <row r="318" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B318" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C318" s="15"/>
+      <c r="D318" s="15"/>
+      <c r="E318" s="15"/>
+      <c r="F318" s="15"/>
+      <c r="G318" s="15"/>
+      <c r="H318" s="15"/>
+      <c r="I318" s="9"/>
+    </row>
+    <row r="319" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B319" s="8"/>
+      <c r="C319" s="15"/>
+      <c r="D319" s="15"/>
+      <c r="E319" s="15"/>
+      <c r="F319" s="15"/>
+      <c r="G319" s="15"/>
+      <c r="H319" s="15"/>
+      <c r="I319" s="9"/>
+    </row>
+    <row r="320" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B320" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C320" s="15"/>
+      <c r="D320" s="15"/>
+      <c r="E320" s="15"/>
+      <c r="F320" s="15"/>
+      <c r="G320" s="15"/>
+      <c r="H320" s="15"/>
+      <c r="I320" s="9"/>
+    </row>
+    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B321" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C321" s="15"/>
+      <c r="D321" s="15"/>
+      <c r="E321" s="15"/>
+      <c r="F321" s="15"/>
+      <c r="G321" s="15"/>
+      <c r="H321" s="15"/>
+      <c r="I321" s="9"/>
+    </row>
+    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B322" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C322" s="15"/>
+      <c r="D322" s="15"/>
+      <c r="E322" s="15"/>
+      <c r="F322" s="15"/>
+      <c r="G322" s="15"/>
+      <c r="H322" s="15"/>
+      <c r="I322" s="9"/>
+    </row>
+    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B323" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C323" s="15"/>
+      <c r="D323" s="15"/>
+      <c r="E323" s="15"/>
+      <c r="F323" s="15"/>
+      <c r="G323" s="15"/>
+      <c r="H323" s="15"/>
+      <c r="I323" s="9"/>
+    </row>
+    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B324" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C324" s="15"/>
+      <c r="D324" s="15"/>
+      <c r="E324" s="15"/>
+      <c r="F324" s="15"/>
+      <c r="G324" s="15"/>
+      <c r="H324" s="15"/>
+      <c r="I324" s="9"/>
+    </row>
+    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B325" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C325" s="15"/>
+      <c r="D325" s="15"/>
+      <c r="E325" s="15"/>
+      <c r="F325" s="15"/>
+      <c r="G325" s="15"/>
+      <c r="H325" s="15"/>
+      <c r="I325" s="9"/>
+    </row>
+    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B326" s="8"/>
+      <c r="C326" s="15"/>
+      <c r="D326" s="15"/>
+      <c r="E326" s="15"/>
+      <c r="F326" s="15"/>
+      <c r="G326" s="15"/>
+      <c r="H326" s="15"/>
+      <c r="I326" s="9"/>
+    </row>
+    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B327" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C327" s="15"/>
+      <c r="D327" s="15"/>
+      <c r="E327" s="15"/>
+      <c r="F327" s="15"/>
+      <c r="G327" s="15"/>
+      <c r="H327" s="15"/>
+      <c r="I327" s="9"/>
+    </row>
+    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B328" s="8"/>
+      <c r="C328" s="15"/>
+      <c r="D328" s="15"/>
+      <c r="E328" s="15"/>
+      <c r="F328" s="15"/>
+      <c r="G328" s="15"/>
+      <c r="H328" s="15"/>
+      <c r="I328" s="9"/>
+    </row>
+    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B329" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C329" s="15"/>
+      <c r="D329" s="15"/>
+      <c r="E329" s="15"/>
+      <c r="F329" s="15"/>
+      <c r="G329" s="15"/>
+      <c r="H329" s="15"/>
+      <c r="I329" s="9"/>
+    </row>
+    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B330" s="8"/>
+      <c r="C330" s="15"/>
+      <c r="D330" s="15"/>
+      <c r="E330" s="15"/>
+      <c r="F330" s="15"/>
+      <c r="G330" s="15"/>
+      <c r="H330" s="15"/>
+      <c r="I330" s="9"/>
+    </row>
+    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B331" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C331" s="11"/>
+      <c r="D331" s="11"/>
+      <c r="E331" s="11"/>
+      <c r="F331" s="11"/>
+      <c r="G331" s="11"/>
+      <c r="H331" s="11"/>
+      <c r="I331" s="13"/>
+    </row>
+    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A334" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B335" s="28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>